<commit_message>
Removed tab from Excel file
There was an additional tab in the Excel file that should not have been there, with calculations in it.
</commit_message>
<xml_diff>
--- a/tacrolimus/2015/25801146-CYP3A5 allele frequency table.xlsx
+++ b/tacrolimus/2015/25801146-CYP3A5 allele frequency table.xlsx
@@ -1,16 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26311"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliabarbarino/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="140" yWindow="0" windowWidth="28660" windowHeight="15640" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="460" windowWidth="28660" windowHeight="15640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1074,7 +1078,7 @@
       <name val="Times New Roman"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1103,12 +1107,6 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFD9D9D9"/>
-        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -1310,7 +1308,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1390,26 +1388,23 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1420,14 +1415,11 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1440,18 +1432,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="82">
@@ -1540,6 +1520,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1867,11 +1852,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A128" workbookViewId="0">
-      <selection activeCell="E131" sqref="E131"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="28" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="9"/>
     <col min="2" max="2" width="18" style="9" customWidth="1"/>
@@ -1882,8 +1867,8 @@
     <col min="10" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="28" customHeight="1">
-      <c r="A1" s="38"/>
+    <row r="1" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="36"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1922,15 +1907,15 @@
       </c>
       <c r="N1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="28" customHeight="1">
-      <c r="A2" s="38"/>
+    <row r="2" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="36"/>
       <c r="B2" s="4" t="s">
         <v>70</v>
       </c>
       <c r="C2" s="4">
         <v>2011</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="27">
         <v>21206424</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -1955,8 +1940,8 @@
       <c r="L2" s="4"/>
       <c r="M2" s="7"/>
     </row>
-    <row r="3" spans="1:14" ht="28" customHeight="1">
-      <c r="A3" s="38"/>
+    <row r="3" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="36"/>
       <c r="B3" s="4" t="s">
         <v>71</v>
       </c>
@@ -1988,8 +1973,8 @@
       <c r="L3" s="4"/>
       <c r="M3" s="7"/>
     </row>
-    <row r="4" spans="1:14" ht="28" customHeight="1">
-      <c r="A4" s="38"/>
+    <row r="4" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="36"/>
       <c r="B4" s="4" t="s">
         <v>72</v>
       </c>
@@ -2021,8 +2006,8 @@
       <c r="L4" s="4"/>
       <c r="M4" s="7"/>
     </row>
-    <row r="5" spans="1:14" ht="28" customHeight="1">
-      <c r="A5" s="38"/>
+    <row r="5" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="36"/>
       <c r="B5" s="4" t="s">
         <v>73</v>
       </c>
@@ -2056,8 +2041,8 @@
       </c>
       <c r="M5" s="7"/>
     </row>
-    <row r="6" spans="1:14" ht="28" customHeight="1">
-      <c r="A6" s="38"/>
+    <row r="6" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="36"/>
       <c r="B6" s="4" t="s">
         <v>74</v>
       </c>
@@ -2091,15 +2076,15 @@
       </c>
       <c r="M6" s="7"/>
     </row>
-    <row r="7" spans="1:14" ht="28" customHeight="1">
-      <c r="A7" s="38"/>
+    <row r="7" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="36"/>
       <c r="B7" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C7" s="4">
         <v>2012</v>
       </c>
-      <c r="D7" s="33">
+      <c r="D7" s="27">
         <v>23128226</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -2128,15 +2113,15 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="28" customHeight="1">
-      <c r="A8" s="38"/>
+    <row r="8" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="36"/>
       <c r="B8" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C8" s="4">
         <v>2003</v>
       </c>
-      <c r="D8" s="33">
+      <c r="D8" s="27">
         <v>14685227</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -2163,8 +2148,8 @@
       </c>
       <c r="M8" s="7"/>
     </row>
-    <row r="9" spans="1:14" ht="28" customHeight="1">
-      <c r="A9" s="38"/>
+    <row r="9" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="36"/>
       <c r="B9" s="4" t="s">
         <v>77</v>
       </c>
@@ -2198,8 +2183,8 @@
       </c>
       <c r="M9" s="7"/>
     </row>
-    <row r="10" spans="1:14" ht="28" customHeight="1">
-      <c r="A10" s="34" t="s">
+    <row r="10" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="33" t="s">
         <v>264</v>
       </c>
       <c r="B10" s="23" t="s">
@@ -2225,8 +2210,8 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="28" customHeight="1">
-      <c r="A11" s="35"/>
+    <row r="11" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="34"/>
       <c r="B11" s="19" t="s">
         <v>259</v>
       </c>
@@ -2250,8 +2235,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="28" customHeight="1">
-      <c r="A12" s="36"/>
+    <row r="12" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="35"/>
       <c r="B12" s="19" t="s">
         <v>261</v>
       </c>
@@ -2275,7 +2260,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="13" spans="1:14" ht="28" customHeight="1">
+    <row r="13" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="37"/>
       <c r="B13" s="4" t="s">
         <v>78</v>
@@ -2308,8 +2293,8 @@
       <c r="L13" s="4"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="1:14" ht="28" customHeight="1">
-      <c r="A14" s="38"/>
+    <row r="14" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="36"/>
       <c r="B14" s="4" t="s">
         <v>79</v>
       </c>
@@ -2347,8 +2332,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28" customHeight="1">
-      <c r="A15" s="38"/>
+    <row r="15" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="36"/>
       <c r="B15" s="4" t="s">
         <v>79</v>
       </c>
@@ -2386,8 +2371,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="28" customHeight="1">
-      <c r="A16" s="38"/>
+    <row r="16" spans="1:14" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="36"/>
       <c r="B16" s="4" t="s">
         <v>79</v>
       </c>
@@ -2425,8 +2410,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="28" customHeight="1">
-      <c r="A17" s="38"/>
+    <row r="17" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="36"/>
       <c r="B17" s="4" t="s">
         <v>79</v>
       </c>
@@ -2464,8 +2449,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="28" customHeight="1">
-      <c r="A18" s="38"/>
+    <row r="18" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="36"/>
       <c r="B18" s="4" t="s">
         <v>79</v>
       </c>
@@ -2503,15 +2488,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="28" customHeight="1">
-      <c r="A19" s="38"/>
+    <row r="19" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="36"/>
       <c r="B19" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C19" s="4">
         <v>2012</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="27">
         <v>23128226</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -2542,15 +2527,15 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="28" customHeight="1">
-      <c r="A20" s="38"/>
+    <row r="20" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="36"/>
       <c r="B20" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C20" s="4">
         <v>2003</v>
       </c>
-      <c r="D20" s="33">
+      <c r="D20" s="27">
         <v>14685227</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -2579,15 +2564,15 @@
       </c>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="1:13" ht="28" customHeight="1">
-      <c r="A21" s="38"/>
+    <row r="21" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="36"/>
       <c r="B21" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C21" s="4">
         <v>2003</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="27">
         <v>14685227</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -2616,8 +2601,8 @@
       </c>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="1:13" ht="28" customHeight="1">
-      <c r="A22" s="38"/>
+    <row r="22" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="36"/>
       <c r="B22" s="4" t="s">
         <v>79</v>
       </c>
@@ -2653,8 +2638,8 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="28" customHeight="1">
-      <c r="A23" s="38"/>
+    <row r="23" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="36"/>
       <c r="B23" s="4" t="s">
         <v>80</v>
       </c>
@@ -2686,8 +2671,8 @@
       <c r="L23" s="4"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="1:13" ht="28" customHeight="1">
-      <c r="A24" s="38"/>
+    <row r="24" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="36"/>
       <c r="B24" s="4" t="s">
         <v>79</v>
       </c>
@@ -2725,8 +2710,8 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="28" customHeight="1">
-      <c r="A25" s="40"/>
+    <row r="25" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="38"/>
       <c r="B25" s="4" t="s">
         <v>79</v>
       </c>
@@ -2764,8 +2749,8 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="28" customHeight="1">
-      <c r="A26" s="34" t="s">
+    <row r="26" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="33" t="s">
         <v>265</v>
       </c>
       <c r="B26" s="23" t="s">
@@ -2791,8 +2776,8 @@
         <v>4.2999999999999997E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="28" customHeight="1">
-      <c r="A27" s="35"/>
+    <row r="27" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="34"/>
       <c r="B27" s="19" t="s">
         <v>259</v>
       </c>
@@ -2816,8 +2801,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="28" customHeight="1">
-      <c r="A28" s="36"/>
+    <row r="28" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="35"/>
       <c r="B28" s="19" t="s">
         <v>261</v>
       </c>
@@ -2841,7 +2826,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="28" customHeight="1">
+    <row r="29" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="37"/>
       <c r="B29" s="4" t="s">
         <v>79</v>
@@ -2880,8 +2865,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="28" customHeight="1">
-      <c r="A30" s="38"/>
+    <row r="30" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="36"/>
       <c r="B30" s="4" t="s">
         <v>81</v>
       </c>
@@ -2913,8 +2898,8 @@
       <c r="L30" s="4"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="1:13" ht="28" customHeight="1">
-      <c r="A31" s="38"/>
+    <row r="31" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="36"/>
       <c r="B31" s="4" t="s">
         <v>79</v>
       </c>
@@ -2952,8 +2937,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="28" customHeight="1">
-      <c r="A32" s="38"/>
+    <row r="32" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="36"/>
       <c r="B32" s="4" t="s">
         <v>79</v>
       </c>
@@ -2991,8 +2976,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="28" customHeight="1">
-      <c r="A33" s="38"/>
+    <row r="33" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="36"/>
       <c r="B33" s="4" t="s">
         <v>79</v>
       </c>
@@ -3030,8 +3015,8 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="28" customHeight="1">
-      <c r="A34" s="38"/>
+    <row r="34" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="36"/>
       <c r="B34" s="4" t="s">
         <v>82</v>
       </c>
@@ -3063,8 +3048,8 @@
       <c r="L34" s="4"/>
       <c r="M34" s="7"/>
     </row>
-    <row r="35" spans="1:13" ht="28" customHeight="1">
-      <c r="A35" s="34" t="s">
+    <row r="35" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
         <v>266</v>
       </c>
       <c r="B35" s="23" t="s">
@@ -3090,8 +3075,8 @@
         <v>7.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="28" customHeight="1">
-      <c r="A36" s="35"/>
+    <row r="36" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="34"/>
       <c r="B36" s="19" t="s">
         <v>259</v>
       </c>
@@ -3115,8 +3100,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="28" customHeight="1">
-      <c r="A37" s="36"/>
+    <row r="37" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="35"/>
       <c r="B37" s="19" t="s">
         <v>261</v>
       </c>
@@ -3140,7 +3125,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="28" customHeight="1">
+    <row r="38" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="37"/>
       <c r="B38" s="15" t="s">
         <v>79</v>
@@ -3179,8 +3164,8 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="28" customHeight="1">
-      <c r="A39" s="38"/>
+    <row r="39" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="36"/>
       <c r="B39" s="15" t="s">
         <v>79</v>
       </c>
@@ -3218,8 +3203,8 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="28" customHeight="1">
-      <c r="A40" s="38"/>
+    <row r="40" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="36"/>
       <c r="B40" s="15" t="s">
         <v>79</v>
       </c>
@@ -3257,8 +3242,8 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="28" customHeight="1">
-      <c r="A41" s="38"/>
+    <row r="41" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="36"/>
       <c r="B41" s="15" t="s">
         <v>79</v>
       </c>
@@ -3296,8 +3281,8 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="28" customHeight="1">
-      <c r="A42" s="38"/>
+    <row r="42" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="36"/>
       <c r="B42" s="15" t="s">
         <v>79</v>
       </c>
@@ -3335,8 +3320,8 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="28" customHeight="1">
-      <c r="A43" s="38"/>
+    <row r="43" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="36"/>
       <c r="B43" s="15" t="s">
         <v>79</v>
       </c>
@@ -3374,8 +3359,8 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="28" customHeight="1">
-      <c r="A44" s="38"/>
+    <row r="44" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="36"/>
       <c r="B44" s="4" t="s">
         <v>83</v>
       </c>
@@ -3407,8 +3392,8 @@
       <c r="L44" s="4"/>
       <c r="M44" s="7"/>
     </row>
-    <row r="45" spans="1:13" ht="28" customHeight="1">
-      <c r="A45" s="38"/>
+    <row r="45" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="36"/>
       <c r="B45" s="4" t="s">
         <v>84</v>
       </c>
@@ -3442,8 +3427,8 @@
       <c r="L45" s="4"/>
       <c r="M45" s="7"/>
     </row>
-    <row r="46" spans="1:13" ht="28" customHeight="1">
-      <c r="A46" s="38"/>
+    <row r="46" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="36"/>
       <c r="B46" s="15" t="s">
         <v>79</v>
       </c>
@@ -3481,8 +3466,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="28" customHeight="1">
-      <c r="A47" s="38"/>
+    <row r="47" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="36"/>
       <c r="B47" s="15" t="s">
         <v>79</v>
       </c>
@@ -3520,8 +3505,8 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="28" customHeight="1">
-      <c r="A48" s="38"/>
+    <row r="48" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="36"/>
       <c r="B48" s="15" t="s">
         <v>79</v>
       </c>
@@ -3559,8 +3544,8 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="28" customHeight="1">
-      <c r="A49" s="34" t="s">
+    <row r="49" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="33" t="s">
         <v>267</v>
       </c>
       <c r="B49" s="23" t="s">
@@ -3586,8 +3571,8 @@
         <v>0.14199999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="28" customHeight="1">
-      <c r="A50" s="35"/>
+    <row r="50" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="34"/>
       <c r="B50" s="19" t="s">
         <v>259</v>
       </c>
@@ -3611,8 +3596,8 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="28" customHeight="1">
-      <c r="A51" s="36"/>
+    <row r="51" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="35"/>
       <c r="B51" s="19" t="s">
         <v>261</v>
       </c>
@@ -3636,7 +3621,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="28" customHeight="1">
+    <row r="52" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="37"/>
       <c r="B52" s="4" t="s">
         <v>85</v>
@@ -3671,8 +3656,8 @@
       </c>
       <c r="M52" s="7"/>
     </row>
-    <row r="53" spans="1:13" ht="28" customHeight="1">
-      <c r="A53" s="38"/>
+    <row r="53" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="36"/>
       <c r="B53" s="15" t="s">
         <v>79</v>
       </c>
@@ -3710,8 +3695,8 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="28" customHeight="1">
-      <c r="A54" s="38"/>
+    <row r="54" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="36"/>
       <c r="B54" s="15" t="s">
         <v>79</v>
       </c>
@@ -3749,8 +3734,8 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="28" customHeight="1">
-      <c r="A55" s="38"/>
+    <row r="55" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="36"/>
       <c r="B55" s="15" t="s">
         <v>79</v>
       </c>
@@ -3788,8 +3773,8 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="28" customHeight="1">
-      <c r="A56" s="38"/>
+    <row r="56" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="36"/>
       <c r="B56" s="15" t="s">
         <v>79</v>
       </c>
@@ -3827,8 +3812,8 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="28" customHeight="1">
-      <c r="A57" s="38"/>
+    <row r="57" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="36"/>
       <c r="B57" s="15" t="s">
         <v>79</v>
       </c>
@@ -3866,8 +3851,8 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="28" customHeight="1">
-      <c r="A58" s="34" t="s">
+    <row r="58" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="33" t="s">
         <v>268</v>
       </c>
       <c r="B58" s="23" t="s">
@@ -3893,8 +3878,8 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="28" customHeight="1">
-      <c r="A59" s="35"/>
+    <row r="59" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="34"/>
       <c r="B59" s="19" t="s">
         <v>259</v>
       </c>
@@ -3918,8 +3903,8 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="28" customHeight="1">
-      <c r="A60" s="36"/>
+    <row r="60" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="35"/>
       <c r="B60" s="19" t="s">
         <v>261</v>
       </c>
@@ -3943,7 +3928,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="28" customHeight="1">
+    <row r="61" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="37"/>
       <c r="B61" s="4" t="s">
         <v>83</v>
@@ -3976,8 +3961,8 @@
       <c r="L61" s="4"/>
       <c r="M61" s="7"/>
     </row>
-    <row r="62" spans="1:13" ht="28" customHeight="1">
-      <c r="A62" s="38"/>
+    <row r="62" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="36"/>
       <c r="B62" s="15" t="s">
         <v>79</v>
       </c>
@@ -4015,8 +4000,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="28" customHeight="1">
-      <c r="A63" s="38"/>
+    <row r="63" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="36"/>
       <c r="B63" s="15" t="s">
         <v>79</v>
       </c>
@@ -4054,8 +4039,8 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="28" customHeight="1">
-      <c r="A64" s="38"/>
+    <row r="64" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="36"/>
       <c r="B64" s="15" t="s">
         <v>79</v>
       </c>
@@ -4093,8 +4078,8 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="28" customHeight="1">
-      <c r="A65" s="38"/>
+    <row r="65" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="36"/>
       <c r="B65" s="15" t="s">
         <v>79</v>
       </c>
@@ -4132,8 +4117,8 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="28" customHeight="1">
-      <c r="A66" s="38"/>
+    <row r="66" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="36"/>
       <c r="B66" s="15" t="s">
         <v>79</v>
       </c>
@@ -4171,8 +4156,8 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="28" customHeight="1">
-      <c r="A67" s="38"/>
+    <row r="67" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="36"/>
       <c r="B67" s="4" t="s">
         <v>82</v>
       </c>
@@ -4204,15 +4189,15 @@
       <c r="L67" s="4"/>
       <c r="M67" s="7"/>
     </row>
-    <row r="68" spans="1:13" ht="28" customHeight="1">
-      <c r="A68" s="38"/>
+    <row r="68" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="36"/>
       <c r="B68" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C68" s="4">
         <v>2012</v>
       </c>
-      <c r="D68" s="33">
+      <c r="D68" s="27">
         <v>23128226</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -4243,15 +4228,15 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="28" customHeight="1">
-      <c r="A69" s="38"/>
+    <row r="69" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="36"/>
       <c r="B69" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C69" s="4">
         <v>2003</v>
       </c>
-      <c r="D69" s="33">
+      <c r="D69" s="27">
         <v>14685227</v>
       </c>
       <c r="E69" s="5" t="s">
@@ -4280,8 +4265,8 @@
       </c>
       <c r="M69" s="7"/>
     </row>
-    <row r="70" spans="1:13" ht="28" customHeight="1">
-      <c r="A70" s="38"/>
+    <row r="70" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="36"/>
       <c r="B70" s="15" t="s">
         <v>79</v>
       </c>
@@ -4319,8 +4304,8 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="28" customHeight="1">
-      <c r="A71" s="38"/>
+    <row r="71" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="36"/>
       <c r="B71" s="4" t="s">
         <v>83</v>
       </c>
@@ -4352,8 +4337,8 @@
       <c r="L71" s="4"/>
       <c r="M71" s="7"/>
     </row>
-    <row r="72" spans="1:13" ht="28" customHeight="1">
-      <c r="A72" s="34" t="s">
+    <row r="72" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="33" t="s">
         <v>269</v>
       </c>
       <c r="B72" s="23" t="s">
@@ -4379,8 +4364,8 @@
         <v>8.6999999999999994E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="28" customHeight="1">
-      <c r="A73" s="35"/>
+    <row r="73" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="34"/>
       <c r="B73" s="19" t="s">
         <v>259</v>
       </c>
@@ -4404,8 +4389,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="28" customHeight="1">
-      <c r="A74" s="36"/>
+    <row r="74" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="35"/>
       <c r="B74" s="19" t="s">
         <v>261</v>
       </c>
@@ -4429,8 +4414,8 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="28" customHeight="1">
-      <c r="A75" s="41" t="s">
+    <row r="75" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="39" t="s">
         <v>270</v>
       </c>
       <c r="B75" s="25" t="s">
@@ -4456,8 +4441,8 @@
         <v>7.6999999999999999E-2</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="28" customHeight="1">
-      <c r="A76" s="42"/>
+    <row r="76" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="40"/>
       <c r="B76" s="21" t="s">
         <v>272</v>
       </c>
@@ -4481,8 +4466,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" ht="28" customHeight="1">
-      <c r="A77" s="43"/>
+    <row r="77" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="41"/>
       <c r="B77" s="21" t="s">
         <v>261</v>
       </c>
@@ -4506,7 +4491,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="28" customHeight="1">
+    <row r="78" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="37"/>
       <c r="B78" s="4" t="s">
         <v>86</v>
@@ -4539,8 +4524,8 @@
       <c r="L78" s="4"/>
       <c r="M78" s="7"/>
     </row>
-    <row r="79" spans="1:13" ht="28" customHeight="1">
-      <c r="A79" s="38"/>
+    <row r="79" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="36"/>
       <c r="B79" s="4" t="s">
         <v>87</v>
       </c>
@@ -4572,8 +4557,8 @@
       <c r="L79" s="4"/>
       <c r="M79" s="7"/>
     </row>
-    <row r="80" spans="1:13" ht="28" customHeight="1">
-      <c r="A80" s="38"/>
+    <row r="80" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="36"/>
       <c r="B80" s="4" t="s">
         <v>88</v>
       </c>
@@ -4605,8 +4590,8 @@
       <c r="L80" s="4"/>
       <c r="M80" s="7"/>
     </row>
-    <row r="81" spans="1:13" ht="28" customHeight="1">
-      <c r="A81" s="38"/>
+    <row r="81" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="36"/>
       <c r="B81" s="4" t="s">
         <v>89</v>
       </c>
@@ -4638,8 +4623,8 @@
       <c r="L81" s="4"/>
       <c r="M81" s="7"/>
     </row>
-    <row r="82" spans="1:13" ht="28" customHeight="1">
-      <c r="A82" s="38"/>
+    <row r="82" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="36"/>
       <c r="B82" s="4" t="s">
         <v>90</v>
       </c>
@@ -4673,15 +4658,15 @@
       </c>
       <c r="M82" s="7"/>
     </row>
-    <row r="83" spans="1:13" ht="28" customHeight="1">
-      <c r="A83" s="38"/>
+    <row r="83" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="36"/>
       <c r="B83" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C83" s="4">
         <v>2014</v>
       </c>
-      <c r="D83" s="33">
+      <c r="D83" s="27">
         <v>24438215</v>
       </c>
       <c r="E83" s="5" t="s">
@@ -4706,8 +4691,8 @@
       <c r="L83" s="4"/>
       <c r="M83" s="7"/>
     </row>
-    <row r="84" spans="1:13" ht="28" customHeight="1">
-      <c r="A84" s="38"/>
+    <row r="84" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="36"/>
       <c r="B84" s="4" t="s">
         <v>92</v>
       </c>
@@ -4739,8 +4724,8 @@
       <c r="L84" s="4"/>
       <c r="M84" s="7"/>
     </row>
-    <row r="85" spans="1:13" ht="28" customHeight="1">
-      <c r="A85" s="38"/>
+    <row r="85" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="36"/>
       <c r="B85" s="4" t="s">
         <v>93</v>
       </c>
@@ -4772,8 +4757,8 @@
       <c r="L85" s="4"/>
       <c r="M85" s="7"/>
     </row>
-    <row r="86" spans="1:13" ht="28" customHeight="1">
-      <c r="A86" s="38"/>
+    <row r="86" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="36"/>
       <c r="B86" s="4" t="s">
         <v>94</v>
       </c>
@@ -4805,8 +4790,8 @@
       <c r="L86" s="4"/>
       <c r="M86" s="7"/>
     </row>
-    <row r="87" spans="1:13" ht="28" customHeight="1">
-      <c r="A87" s="38"/>
+    <row r="87" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="36"/>
       <c r="B87" s="4" t="s">
         <v>86</v>
       </c>
@@ -4838,15 +4823,15 @@
       <c r="L87" s="4"/>
       <c r="M87" s="7"/>
     </row>
-    <row r="88" spans="1:13" ht="28" customHeight="1">
-      <c r="A88" s="38"/>
+    <row r="88" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="36"/>
       <c r="B88" s="4" t="s">
         <v>92</v>
       </c>
       <c r="C88" s="4">
         <v>2013</v>
       </c>
-      <c r="D88" s="33">
+      <c r="D88" s="27">
         <v>23459029</v>
       </c>
       <c r="E88" s="5" t="s">
@@ -4871,8 +4856,8 @@
       <c r="L88" s="4"/>
       <c r="M88" s="7"/>
     </row>
-    <row r="89" spans="1:13" ht="28" customHeight="1">
-      <c r="A89" s="38"/>
+    <row r="89" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="36"/>
       <c r="B89" s="4" t="s">
         <v>95</v>
       </c>
@@ -4904,8 +4889,8 @@
       <c r="L89" s="4"/>
       <c r="M89" s="7"/>
     </row>
-    <row r="90" spans="1:13" ht="28" customHeight="1">
-      <c r="A90" s="38"/>
+    <row r="90" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="36"/>
       <c r="B90" s="4" t="s">
         <v>95</v>
       </c>
@@ -4937,8 +4922,8 @@
       <c r="L90" s="4"/>
       <c r="M90" s="7"/>
     </row>
-    <row r="91" spans="1:13" ht="28" customHeight="1">
-      <c r="A91" s="38"/>
+    <row r="91" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="36"/>
       <c r="B91" s="4" t="s">
         <v>96</v>
       </c>
@@ -4970,8 +4955,8 @@
       <c r="L91" s="4"/>
       <c r="M91" s="7"/>
     </row>
-    <row r="92" spans="1:13" ht="28" customHeight="1">
-      <c r="A92" s="38"/>
+    <row r="92" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="36"/>
       <c r="B92" s="4" t="s">
         <v>86</v>
       </c>
@@ -5003,8 +4988,8 @@
       <c r="L92" s="4"/>
       <c r="M92" s="7"/>
     </row>
-    <row r="93" spans="1:13" ht="28" customHeight="1">
-      <c r="A93" s="38"/>
+    <row r="93" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="36"/>
       <c r="B93" s="4" t="s">
         <v>97</v>
       </c>
@@ -5036,8 +5021,8 @@
       <c r="L93" s="4"/>
       <c r="M93" s="7"/>
     </row>
-    <row r="94" spans="1:13" ht="28" customHeight="1">
-      <c r="A94" s="38"/>
+    <row r="94" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="36"/>
       <c r="B94" s="4" t="s">
         <v>86</v>
       </c>
@@ -5069,8 +5054,8 @@
       <c r="L94" s="4"/>
       <c r="M94" s="7"/>
     </row>
-    <row r="95" spans="1:13" ht="28" customHeight="1">
-      <c r="A95" s="38"/>
+    <row r="95" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="36"/>
       <c r="B95" s="4" t="s">
         <v>96</v>
       </c>
@@ -5102,8 +5087,8 @@
       <c r="L95" s="4"/>
       <c r="M95" s="7"/>
     </row>
-    <row r="96" spans="1:13" ht="28" customHeight="1">
-      <c r="A96" s="38"/>
+    <row r="96" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="36"/>
       <c r="B96" s="4" t="s">
         <v>86</v>
       </c>
@@ -5135,8 +5120,8 @@
       <c r="L96" s="4"/>
       <c r="M96" s="7"/>
     </row>
-    <row r="97" spans="1:13" ht="28" customHeight="1">
-      <c r="A97" s="38"/>
+    <row r="97" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="36"/>
       <c r="B97" s="4" t="s">
         <v>86</v>
       </c>
@@ -5168,8 +5153,8 @@
       <c r="L97" s="4"/>
       <c r="M97" s="7"/>
     </row>
-    <row r="98" spans="1:13" ht="28" customHeight="1">
-      <c r="A98" s="38"/>
+    <row r="98" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98" s="36"/>
       <c r="B98" s="4" t="s">
         <v>98</v>
       </c>
@@ -5201,8 +5186,8 @@
       <c r="L98" s="4"/>
       <c r="M98" s="7"/>
     </row>
-    <row r="99" spans="1:13" ht="28" customHeight="1">
-      <c r="A99" s="38"/>
+    <row r="99" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="36"/>
       <c r="B99" s="4" t="s">
         <v>99</v>
       </c>
@@ -5234,15 +5219,15 @@
       <c r="L99" s="4"/>
       <c r="M99" s="7"/>
     </row>
-    <row r="100" spans="1:13" ht="28" customHeight="1">
-      <c r="A100" s="38"/>
+    <row r="100" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="36"/>
       <c r="B100" s="4" t="s">
         <v>96</v>
       </c>
       <c r="C100" s="4">
         <v>2005</v>
       </c>
-      <c r="D100" s="33">
+      <c r="D100" s="27">
         <v>16146556</v>
       </c>
       <c r="E100" s="5" t="s">
@@ -5267,8 +5252,8 @@
       <c r="L100" s="4"/>
       <c r="M100" s="7"/>
     </row>
-    <row r="101" spans="1:13" ht="28" customHeight="1">
-      <c r="A101" s="38"/>
+    <row r="101" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="36"/>
       <c r="B101" s="4" t="s">
         <v>100</v>
       </c>
@@ -5300,8 +5285,8 @@
       <c r="L101" s="4"/>
       <c r="M101" s="7"/>
     </row>
-    <row r="102" spans="1:13" ht="28" customHeight="1">
-      <c r="A102" s="38"/>
+    <row r="102" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A102" s="36"/>
       <c r="B102" s="4" t="s">
         <v>91</v>
       </c>
@@ -5333,8 +5318,8 @@
       <c r="L102" s="4"/>
       <c r="M102" s="7"/>
     </row>
-    <row r="103" spans="1:13" ht="28" customHeight="1">
-      <c r="A103" s="38"/>
+    <row r="103" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="36"/>
       <c r="B103" s="4" t="s">
         <v>101</v>
       </c>
@@ -5366,8 +5351,8 @@
       <c r="L103" s="4"/>
       <c r="M103" s="7"/>
     </row>
-    <row r="104" spans="1:13" ht="28" customHeight="1">
-      <c r="A104" s="38"/>
+    <row r="104" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="36"/>
       <c r="B104" s="4" t="s">
         <v>100</v>
       </c>
@@ -5399,8 +5384,8 @@
       <c r="L104" s="4"/>
       <c r="M104" s="7"/>
     </row>
-    <row r="105" spans="1:13" ht="28" customHeight="1">
-      <c r="A105" s="38"/>
+    <row r="105" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="36"/>
       <c r="B105" s="4" t="s">
         <v>102</v>
       </c>
@@ -5436,15 +5421,15 @@
       </c>
       <c r="M105" s="7"/>
     </row>
-    <row r="106" spans="1:13" ht="28" customHeight="1">
-      <c r="A106" s="38"/>
+    <row r="106" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="36"/>
       <c r="B106" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C106" s="4">
         <v>2012</v>
       </c>
-      <c r="D106" s="33">
+      <c r="D106" s="27">
         <v>23128226</v>
       </c>
       <c r="E106" s="5" t="s">
@@ -5475,15 +5460,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="28" customHeight="1">
-      <c r="A107" s="38"/>
+    <row r="107" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="36"/>
       <c r="B107" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C107" s="4">
         <v>2012</v>
       </c>
-      <c r="D107" s="33">
+      <c r="D107" s="27">
         <v>23128226</v>
       </c>
       <c r="E107" s="5" t="s">
@@ -5514,15 +5499,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="28" customHeight="1">
-      <c r="A108" s="38"/>
+    <row r="108" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="36"/>
       <c r="B108" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C108" s="4">
         <v>2003</v>
       </c>
-      <c r="D108" s="33">
+      <c r="D108" s="27">
         <v>14685227</v>
       </c>
       <c r="E108" s="5" t="s">
@@ -5551,15 +5536,15 @@
       </c>
       <c r="M108" s="7"/>
     </row>
-    <row r="109" spans="1:13" ht="28" customHeight="1">
-      <c r="A109" s="38"/>
+    <row r="109" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="36"/>
       <c r="B109" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C109" s="4">
         <v>2003</v>
       </c>
-      <c r="D109" s="33">
+      <c r="D109" s="27">
         <v>14685227</v>
       </c>
       <c r="E109" s="5" t="s">
@@ -5586,8 +5571,8 @@
       <c r="L109" s="4"/>
       <c r="M109" s="7"/>
     </row>
-    <row r="110" spans="1:13" ht="28" customHeight="1">
-      <c r="A110" s="38"/>
+    <row r="110" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="36"/>
       <c r="B110" s="4" t="s">
         <v>86</v>
       </c>
@@ -5621,8 +5606,8 @@
       <c r="L110" s="4"/>
       <c r="M110" s="7"/>
     </row>
-    <row r="111" spans="1:13" ht="28" customHeight="1">
-      <c r="A111" s="38"/>
+    <row r="111" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="36"/>
       <c r="B111" s="4" t="s">
         <v>86</v>
       </c>
@@ -5656,8 +5641,8 @@
       <c r="L111" s="4"/>
       <c r="M111" s="7"/>
     </row>
-    <row r="112" spans="1:13" ht="28" customHeight="1">
-      <c r="A112" s="38"/>
+    <row r="112" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="36"/>
       <c r="B112" s="4" t="s">
         <v>103</v>
       </c>
@@ -5691,107 +5676,107 @@
       <c r="L112" s="4"/>
       <c r="M112" s="7"/>
     </row>
-    <row r="113" spans="1:13" s="46" customFormat="1" ht="28" customHeight="1">
-      <c r="A113" s="38"/>
-      <c r="B113" s="44" t="s">
+    <row r="113" spans="1:13" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="36"/>
+      <c r="B113" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="C113" s="44">
+      <c r="C113" s="28">
         <v>2014</v>
       </c>
-      <c r="D113" s="44">
+      <c r="D113" s="28">
         <v>25310192</v>
       </c>
-      <c r="E113" s="45" t="s">
+      <c r="E113" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F113" s="45" t="s">
+      <c r="F113" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G113" s="45"/>
-      <c r="H113" s="45" t="s">
+      <c r="G113" s="29"/>
+      <c r="H113" s="29" t="s">
         <v>284</v>
       </c>
-      <c r="I113" s="45">
+      <c r="I113" s="29">
         <v>180</v>
       </c>
-      <c r="J113" s="45">
+      <c r="J113" s="29">
         <v>0.23899999999999999</v>
       </c>
-      <c r="K113" s="44">
+      <c r="K113" s="28">
         <v>0.76100000000000001</v>
       </c>
-      <c r="L113" s="44"/>
-      <c r="M113" s="44"/>
-    </row>
-    <row r="114" spans="1:13" s="46" customFormat="1" ht="28" customHeight="1">
-      <c r="A114" s="38"/>
-      <c r="B114" s="44" t="s">
+      <c r="L113" s="28"/>
+      <c r="M113" s="28"/>
+    </row>
+    <row r="114" spans="1:13" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="36"/>
+      <c r="B114" s="28" t="s">
         <v>295</v>
       </c>
-      <c r="C114" s="44">
+      <c r="C114" s="28">
         <v>2015</v>
       </c>
-      <c r="D114" s="44">
+      <c r="D114" s="28">
         <v>25487141</v>
       </c>
-      <c r="E114" s="45" t="s">
+      <c r="E114" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F114" s="45" t="s">
+      <c r="F114" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G114" s="45"/>
-      <c r="H114" s="45" t="s">
+      <c r="G114" s="29"/>
+      <c r="H114" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="I114" s="45">
+      <c r="I114" s="29">
         <v>166</v>
       </c>
-      <c r="J114" s="45">
+      <c r="J114" s="29">
         <v>0.3</v>
       </c>
-      <c r="K114" s="44">
+      <c r="K114" s="28">
         <v>0.7</v>
       </c>
-      <c r="L114" s="44"/>
-      <c r="M114" s="44"/>
-    </row>
-    <row r="115" spans="1:13" s="46" customFormat="1" ht="28" customHeight="1">
-      <c r="A115" s="38"/>
-      <c r="B115" s="44" t="s">
+      <c r="L114" s="28"/>
+      <c r="M114" s="28"/>
+    </row>
+    <row r="115" spans="1:13" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="36"/>
+      <c r="B115" s="28" t="s">
         <v>296</v>
       </c>
-      <c r="C115" s="44">
+      <c r="C115" s="28">
         <v>2014</v>
       </c>
-      <c r="D115" s="44">
+      <c r="D115" s="28">
         <v>24820765</v>
       </c>
-      <c r="E115" s="45" t="s">
+      <c r="E115" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F115" s="45" t="s">
+      <c r="F115" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="G115" s="45"/>
-      <c r="H115" s="45" t="s">
+      <c r="G115" s="29"/>
+      <c r="H115" s="29" t="s">
         <v>284</v>
       </c>
-      <c r="I115" s="45">
+      <c r="I115" s="29">
         <v>96</v>
       </c>
-      <c r="J115" s="45">
+      <c r="J115" s="29">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K115" s="44">
+      <c r="K115" s="28">
         <v>0.72</v>
       </c>
-      <c r="L115" s="44"/>
-      <c r="M115" s="44"/>
-    </row>
-    <row r="116" spans="1:13" ht="28" customHeight="1">
-      <c r="A116" s="38"/>
+      <c r="L115" s="28"/>
+      <c r="M115" s="28"/>
+    </row>
+    <row r="116" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A116" s="36"/>
       <c r="B116" s="4" t="s">
         <v>104</v>
       </c>
@@ -5823,8 +5808,8 @@
       <c r="L116" s="4"/>
       <c r="M116" s="7"/>
     </row>
-    <row r="117" spans="1:13" ht="28" customHeight="1">
-      <c r="A117" s="38"/>
+    <row r="117" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A117" s="36"/>
       <c r="B117" s="4" t="s">
         <v>105</v>
       </c>
@@ -5858,8 +5843,8 @@
       </c>
       <c r="M117" s="7"/>
     </row>
-    <row r="118" spans="1:13" ht="28" customHeight="1">
-      <c r="A118" s="38"/>
+    <row r="118" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A118" s="36"/>
       <c r="B118" s="4" t="s">
         <v>106</v>
       </c>
@@ -5891,8 +5876,8 @@
       <c r="L118" s="4"/>
       <c r="M118" s="7"/>
     </row>
-    <row r="119" spans="1:13" ht="28" customHeight="1">
-      <c r="A119" s="38"/>
+    <row r="119" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119" s="36"/>
       <c r="B119" s="4" t="s">
         <v>107</v>
       </c>
@@ -5924,8 +5909,8 @@
       <c r="L119" s="4"/>
       <c r="M119" s="7"/>
     </row>
-    <row r="120" spans="1:13" ht="28" customHeight="1">
-      <c r="A120" s="38"/>
+    <row r="120" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="36"/>
       <c r="B120" s="4" t="s">
         <v>108</v>
       </c>
@@ -5957,8 +5942,8 @@
       <c r="L120" s="4"/>
       <c r="M120" s="7"/>
     </row>
-    <row r="121" spans="1:13" ht="28" customHeight="1">
-      <c r="A121" s="38"/>
+    <row r="121" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121" s="36"/>
       <c r="B121" s="4" t="s">
         <v>107</v>
       </c>
@@ -5990,8 +5975,8 @@
       <c r="L121" s="4"/>
       <c r="M121" s="7"/>
     </row>
-    <row r="122" spans="1:13" ht="28" customHeight="1">
-      <c r="A122" s="38"/>
+    <row r="122" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122" s="36"/>
       <c r="B122" s="4" t="s">
         <v>109</v>
       </c>
@@ -6023,8 +6008,8 @@
       <c r="L122" s="4"/>
       <c r="M122" s="7"/>
     </row>
-    <row r="123" spans="1:13" ht="28" customHeight="1">
-      <c r="A123" s="38"/>
+    <row r="123" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="36"/>
       <c r="B123" s="4" t="s">
         <v>129</v>
       </c>
@@ -6056,8 +6041,8 @@
       <c r="L123" s="4"/>
       <c r="M123" s="7"/>
     </row>
-    <row r="124" spans="1:13" ht="28" customHeight="1">
-      <c r="A124" s="38"/>
+    <row r="124" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="36"/>
       <c r="B124" s="4" t="s">
         <v>110</v>
       </c>
@@ -6089,8 +6074,8 @@
       <c r="L124" s="4"/>
       <c r="M124" s="7"/>
     </row>
-    <row r="125" spans="1:13" ht="28" customHeight="1">
-      <c r="A125" s="38"/>
+    <row r="125" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125" s="36"/>
       <c r="B125" s="4" t="s">
         <v>110</v>
       </c>
@@ -6122,8 +6107,8 @@
       <c r="L125" s="4"/>
       <c r="M125" s="7"/>
     </row>
-    <row r="126" spans="1:13" ht="28" customHeight="1">
-      <c r="A126" s="38"/>
+    <row r="126" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126" s="36"/>
       <c r="B126" s="4" t="s">
         <v>111</v>
       </c>
@@ -6155,8 +6140,8 @@
       <c r="L126" s="4"/>
       <c r="M126" s="7"/>
     </row>
-    <row r="127" spans="1:13" ht="28" customHeight="1">
-      <c r="A127" s="38"/>
+    <row r="127" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A127" s="36"/>
       <c r="B127" s="4" t="s">
         <v>112</v>
       </c>
@@ -6188,8 +6173,8 @@
       <c r="L127" s="4"/>
       <c r="M127" s="7"/>
     </row>
-    <row r="128" spans="1:13" ht="28" customHeight="1">
-      <c r="A128" s="38"/>
+    <row r="128" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A128" s="36"/>
       <c r="B128" s="4" t="s">
         <v>113</v>
       </c>
@@ -6221,8 +6206,8 @@
       <c r="L128" s="4"/>
       <c r="M128" s="7"/>
     </row>
-    <row r="129" spans="1:13" ht="28" customHeight="1">
-      <c r="A129" s="38"/>
+    <row r="129" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="36"/>
       <c r="B129" s="4" t="s">
         <v>114</v>
       </c>
@@ -6254,8 +6239,8 @@
       <c r="L129" s="4"/>
       <c r="M129" s="7"/>
     </row>
-    <row r="130" spans="1:13" ht="28" customHeight="1">
-      <c r="A130" s="38"/>
+    <row r="130" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="36"/>
       <c r="B130" s="4" t="s">
         <v>115</v>
       </c>
@@ -6287,8 +6272,8 @@
       <c r="L130" s="4"/>
       <c r="M130" s="7"/>
     </row>
-    <row r="131" spans="1:13" ht="28" customHeight="1">
-      <c r="A131" s="38"/>
+    <row r="131" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="36"/>
       <c r="B131" s="4" t="s">
         <v>116</v>
       </c>
@@ -6320,8 +6305,8 @@
       <c r="L131" s="4"/>
       <c r="M131" s="7"/>
     </row>
-    <row r="132" spans="1:13" ht="28" customHeight="1">
-      <c r="A132" s="38"/>
+    <row r="132" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="36"/>
       <c r="B132" s="4" t="s">
         <v>117</v>
       </c>
@@ -6353,15 +6338,15 @@
       <c r="L132" s="4"/>
       <c r="M132" s="7"/>
     </row>
-    <row r="133" spans="1:13" ht="28" customHeight="1">
-      <c r="A133" s="38"/>
+    <row r="133" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="36"/>
       <c r="B133" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C133" s="4">
         <v>2012</v>
       </c>
-      <c r="D133" s="33">
+      <c r="D133" s="27">
         <v>23128226</v>
       </c>
       <c r="E133" s="5" t="s">
@@ -6392,15 +6377,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="28" customHeight="1">
-      <c r="A134" s="38"/>
+    <row r="134" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="36"/>
       <c r="B134" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C134" s="4">
         <v>2003</v>
       </c>
-      <c r="D134" s="33">
+      <c r="D134" s="27">
         <v>14685227</v>
       </c>
       <c r="E134" s="5" t="s">
@@ -6429,41 +6414,41 @@
       </c>
       <c r="M134" s="7"/>
     </row>
-    <row r="135" spans="1:13" s="46" customFormat="1" ht="28" customHeight="1">
-      <c r="A135" s="38"/>
-      <c r="B135" s="45" t="s">
+    <row r="135" spans="1:13" s="30" customFormat="1" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="36"/>
+      <c r="B135" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="C135" s="44">
+      <c r="C135" s="28">
         <v>2014</v>
       </c>
-      <c r="D135" s="47">
+      <c r="D135" s="31">
         <v>25594874</v>
       </c>
-      <c r="E135" s="45" t="s">
+      <c r="E135" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="F135" s="45" t="s">
+      <c r="F135" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="G135" s="45"/>
-      <c r="H135" s="45" t="s">
+      <c r="G135" s="29"/>
+      <c r="H135" s="29" t="s">
         <v>283</v>
       </c>
-      <c r="I135" s="45">
+      <c r="I135" s="29">
         <v>50</v>
       </c>
-      <c r="J135" s="45">
+      <c r="J135" s="29">
         <v>0.21</v>
       </c>
-      <c r="K135" s="44">
+      <c r="K135" s="28">
         <v>0.79</v>
       </c>
-      <c r="L135" s="45"/>
-      <c r="M135" s="44"/>
-    </row>
-    <row r="136" spans="1:13" ht="28" customHeight="1">
-      <c r="A136" s="38"/>
+      <c r="L135" s="29"/>
+      <c r="M135" s="28"/>
+    </row>
+    <row r="136" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="36"/>
       <c r="B136" s="4" t="s">
         <v>118</v>
       </c>
@@ -6495,8 +6480,8 @@
       <c r="L136" s="4"/>
       <c r="M136" s="7"/>
     </row>
-    <row r="137" spans="1:13" ht="28" customHeight="1">
-      <c r="A137" s="38"/>
+    <row r="137" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="36"/>
       <c r="B137" s="4" t="s">
         <v>128</v>
       </c>
@@ -6528,8 +6513,8 @@
       <c r="L137" s="4"/>
       <c r="M137" s="7"/>
     </row>
-    <row r="138" spans="1:13" ht="28" customHeight="1">
-      <c r="A138" s="38"/>
+    <row r="138" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="36"/>
       <c r="B138" s="4" t="s">
         <v>118</v>
       </c>
@@ -6561,8 +6546,8 @@
       <c r="L138" s="4"/>
       <c r="M138" s="7"/>
     </row>
-    <row r="139" spans="1:13" ht="28" customHeight="1">
-      <c r="A139" s="38"/>
+    <row r="139" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="36"/>
       <c r="B139" s="4" t="s">
         <v>119</v>
       </c>
@@ -6598,15 +6583,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="28" customHeight="1">
-      <c r="A140" s="38"/>
+    <row r="140" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="36"/>
       <c r="B140" s="4" t="s">
         <v>118</v>
       </c>
       <c r="C140" s="4">
         <v>2012</v>
       </c>
-      <c r="D140" s="33">
+      <c r="D140" s="27">
         <v>22469198</v>
       </c>
       <c r="E140" s="5" t="s">
@@ -6631,8 +6616,8 @@
       <c r="L140" s="4"/>
       <c r="M140" s="7"/>
     </row>
-    <row r="141" spans="1:13" ht="28" customHeight="1">
-      <c r="A141" s="38"/>
+    <row r="141" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="36"/>
       <c r="B141" s="4" t="s">
         <v>120</v>
       </c>
@@ -6664,8 +6649,8 @@
       <c r="L141" s="4"/>
       <c r="M141" s="7"/>
     </row>
-    <row r="142" spans="1:13" ht="28" customHeight="1">
-      <c r="A142" s="38"/>
+    <row r="142" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="36"/>
       <c r="B142" s="4" t="s">
         <v>121</v>
       </c>
@@ -6697,8 +6682,8 @@
       <c r="L142" s="4"/>
       <c r="M142" s="7"/>
     </row>
-    <row r="143" spans="1:13" ht="28" customHeight="1">
-      <c r="A143" s="38"/>
+    <row r="143" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="36"/>
       <c r="B143" s="4" t="s">
         <v>118</v>
       </c>
@@ -6730,8 +6715,8 @@
       <c r="L143" s="4"/>
       <c r="M143" s="7"/>
     </row>
-    <row r="144" spans="1:13" ht="28" customHeight="1">
-      <c r="A144" s="38"/>
+    <row r="144" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="36"/>
       <c r="B144" s="4" t="s">
         <v>122</v>
       </c>
@@ -6763,8 +6748,8 @@
       <c r="L144" s="4"/>
       <c r="M144" s="7"/>
     </row>
-    <row r="145" spans="1:13" ht="28" customHeight="1">
-      <c r="A145" s="38"/>
+    <row r="145" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="36"/>
       <c r="B145" s="4" t="s">
         <v>123</v>
       </c>
@@ -6796,8 +6781,8 @@
       <c r="L145" s="4"/>
       <c r="M145" s="7"/>
     </row>
-    <row r="146" spans="1:13" ht="28" customHeight="1">
-      <c r="A146" s="38"/>
+    <row r="146" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="36"/>
       <c r="B146" s="4" t="s">
         <v>124</v>
       </c>
@@ -6829,8 +6814,8 @@
       <c r="L146" s="4"/>
       <c r="M146" s="7"/>
     </row>
-    <row r="147" spans="1:13" ht="28" customHeight="1">
-      <c r="A147" s="38"/>
+    <row r="147" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="36"/>
       <c r="B147" s="4" t="s">
         <v>125</v>
       </c>
@@ -6862,8 +6847,8 @@
       <c r="L147" s="4"/>
       <c r="M147" s="7"/>
     </row>
-    <row r="148" spans="1:13" ht="28" customHeight="1">
-      <c r="A148" s="38"/>
+    <row r="148" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="36"/>
       <c r="B148" s="4" t="s">
         <v>126</v>
       </c>
@@ -6895,8 +6880,8 @@
       <c r="L148" s="4"/>
       <c r="M148" s="7"/>
     </row>
-    <row r="149" spans="1:13" ht="28" customHeight="1">
-      <c r="A149" s="38"/>
+    <row r="149" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="36"/>
       <c r="B149" s="4" t="s">
         <v>122</v>
       </c>
@@ -6928,8 +6913,8 @@
       <c r="L149" s="4"/>
       <c r="M149" s="7"/>
     </row>
-    <row r="150" spans="1:13" ht="28" customHeight="1">
-      <c r="A150" s="38"/>
+    <row r="150" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="36"/>
       <c r="B150" s="4" t="s">
         <v>127</v>
       </c>
@@ -6961,8 +6946,8 @@
       <c r="L150" s="4"/>
       <c r="M150" s="7"/>
     </row>
-    <row r="151" spans="1:13" ht="28" customHeight="1">
-      <c r="A151" s="38"/>
+    <row r="151" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="36"/>
       <c r="B151" s="4" t="s">
         <v>90</v>
       </c>
@@ -6996,8 +6981,8 @@
       </c>
       <c r="M151" s="7"/>
     </row>
-    <row r="152" spans="1:13" ht="28" customHeight="1">
-      <c r="A152" s="38"/>
+    <row r="152" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="36"/>
       <c r="B152" s="4" t="s">
         <v>93</v>
       </c>
@@ -7029,8 +7014,8 @@
       <c r="L152" s="4"/>
       <c r="M152" s="7"/>
     </row>
-    <row r="153" spans="1:13" ht="28" customHeight="1">
-      <c r="A153" s="38"/>
+    <row r="153" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="36"/>
       <c r="B153" s="4" t="s">
         <v>130</v>
       </c>
@@ -7062,8 +7047,8 @@
       <c r="L153" s="4"/>
       <c r="M153" s="7"/>
     </row>
-    <row r="154" spans="1:13" ht="28" customHeight="1">
-      <c r="A154" s="34" t="s">
+    <row r="154" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="33" t="s">
         <v>273</v>
       </c>
       <c r="B154" s="23" t="s">
@@ -7089,8 +7074,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="28" customHeight="1">
-      <c r="A155" s="35"/>
+    <row r="155" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="34"/>
       <c r="B155" s="19" t="s">
         <v>259</v>
       </c>
@@ -7114,8 +7099,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="28" customHeight="1">
-      <c r="A156" s="36"/>
+    <row r="156" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="35"/>
       <c r="B156" s="19" t="s">
         <v>261</v>
       </c>
@@ -7139,7 +7124,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="28" customHeight="1">
+    <row r="157" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="37"/>
       <c r="B157" s="4" t="s">
         <v>72</v>
@@ -7172,15 +7157,15 @@
       <c r="L157" s="4"/>
       <c r="M157" s="7"/>
     </row>
-    <row r="158" spans="1:13" ht="28" customHeight="1">
-      <c r="A158" s="38"/>
+    <row r="158" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="36"/>
       <c r="B158" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C158" s="4">
         <v>2012</v>
       </c>
-      <c r="D158" s="33">
+      <c r="D158" s="27">
         <v>23128226</v>
       </c>
       <c r="E158" s="5" t="s">
@@ -7209,15 +7194,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:13" ht="28" customHeight="1">
-      <c r="A159" s="38"/>
+    <row r="159" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="36"/>
       <c r="B159" s="5" t="s">
         <v>76</v>
       </c>
       <c r="C159" s="5">
         <v>2003</v>
       </c>
-      <c r="D159" s="33">
+      <c r="D159" s="27">
         <v>14685227</v>
       </c>
       <c r="E159" s="5" t="s">
@@ -7242,8 +7227,8 @@
       <c r="L159" s="5"/>
       <c r="M159" s="7"/>
     </row>
-    <row r="160" spans="1:13" ht="28" customHeight="1">
-      <c r="A160" s="38"/>
+    <row r="160" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="36"/>
       <c r="B160" s="4" t="s">
         <v>131</v>
       </c>
@@ -7275,8 +7260,8 @@
       <c r="L160" s="4"/>
       <c r="M160" s="7"/>
     </row>
-    <row r="161" spans="1:13" ht="28" customHeight="1">
-      <c r="A161" s="38"/>
+    <row r="161" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="36"/>
       <c r="B161" s="4" t="s">
         <v>132</v>
       </c>
@@ -7308,8 +7293,8 @@
       <c r="L161" s="4"/>
       <c r="M161" s="7"/>
     </row>
-    <row r="162" spans="1:13" ht="28" customHeight="1">
-      <c r="A162" s="38"/>
+    <row r="162" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="36"/>
       <c r="B162" s="4" t="s">
         <v>133</v>
       </c>
@@ -7341,8 +7326,8 @@
       <c r="L162" s="4"/>
       <c r="M162" s="7"/>
     </row>
-    <row r="163" spans="1:13" ht="28" customHeight="1">
-      <c r="A163" s="38"/>
+    <row r="163" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="36"/>
       <c r="B163" s="4" t="s">
         <v>134</v>
       </c>
@@ -7374,8 +7359,8 @@
       <c r="L163" s="4"/>
       <c r="M163" s="7"/>
     </row>
-    <row r="164" spans="1:13" ht="28" customHeight="1">
-      <c r="A164" s="38"/>
+    <row r="164" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="36"/>
       <c r="B164" s="4" t="s">
         <v>135</v>
       </c>
@@ -7407,15 +7392,15 @@
       <c r="L164" s="4"/>
       <c r="M164" s="7"/>
     </row>
-    <row r="165" spans="1:13" ht="28" customHeight="1">
-      <c r="A165" s="38"/>
+    <row r="165" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="36"/>
       <c r="B165" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C165" s="4">
         <v>2012</v>
       </c>
-      <c r="D165" s="33">
+      <c r="D165" s="27">
         <v>23128226</v>
       </c>
       <c r="E165" s="5" t="s">
@@ -7444,8 +7429,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:13" ht="28" customHeight="1">
-      <c r="A166" s="38"/>
+    <row r="166" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="36"/>
       <c r="B166" s="4" t="s">
         <v>136</v>
       </c>
@@ -7479,8 +7464,8 @@
       </c>
       <c r="M166" s="7"/>
     </row>
-    <row r="167" spans="1:13" ht="28" customHeight="1">
-      <c r="A167" s="38"/>
+    <row r="167" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="36"/>
       <c r="B167" s="4" t="s">
         <v>137</v>
       </c>
@@ -7516,8 +7501,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:13" ht="28" customHeight="1">
-      <c r="A168" s="38"/>
+    <row r="168" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="36"/>
       <c r="B168" s="4" t="s">
         <v>138</v>
       </c>
@@ -7553,8 +7538,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:13" ht="28" customHeight="1">
-      <c r="A169" s="38"/>
+    <row r="169" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="36"/>
       <c r="B169" s="4" t="s">
         <v>139</v>
       </c>
@@ -7586,8 +7571,8 @@
       <c r="L169" s="4"/>
       <c r="M169" s="7"/>
     </row>
-    <row r="170" spans="1:13" ht="28" customHeight="1">
-      <c r="A170" s="38"/>
+    <row r="170" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="36"/>
       <c r="B170" s="4" t="s">
         <v>74</v>
       </c>
@@ -7621,8 +7606,8 @@
       </c>
       <c r="M170" s="7"/>
     </row>
-    <row r="171" spans="1:13" ht="28" customHeight="1">
-      <c r="A171" s="38"/>
+    <row r="171" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="36"/>
       <c r="B171" s="4" t="s">
         <v>140</v>
       </c>
@@ -7654,15 +7639,15 @@
       <c r="L171" s="4"/>
       <c r="M171" s="7"/>
     </row>
-    <row r="172" spans="1:13" ht="28" customHeight="1">
-      <c r="A172" s="38"/>
+    <row r="172" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="36"/>
       <c r="B172" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C172" s="4">
         <v>2012</v>
       </c>
-      <c r="D172" s="33">
+      <c r="D172" s="27">
         <v>23128226</v>
       </c>
       <c r="E172" s="5" t="s">
@@ -7691,8 +7676,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:13" ht="28" customHeight="1">
-      <c r="A173" s="38"/>
+    <row r="173" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="36"/>
       <c r="B173" s="4" t="s">
         <v>82</v>
       </c>
@@ -7724,8 +7709,8 @@
       <c r="L173" s="4"/>
       <c r="M173" s="7"/>
     </row>
-    <row r="174" spans="1:13" ht="28" customHeight="1">
-      <c r="A174" s="38"/>
+    <row r="174" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="36"/>
       <c r="B174" s="4" t="s">
         <v>94</v>
       </c>
@@ -7757,8 +7742,8 @@
       <c r="L174" s="4"/>
       <c r="M174" s="7"/>
     </row>
-    <row r="175" spans="1:13" ht="28" customHeight="1">
-      <c r="A175" s="38"/>
+    <row r="175" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="36"/>
       <c r="B175" s="4" t="s">
         <v>141</v>
       </c>
@@ -7790,8 +7775,8 @@
       <c r="L175" s="4"/>
       <c r="M175" s="7"/>
     </row>
-    <row r="176" spans="1:13" ht="28" customHeight="1">
-      <c r="A176" s="38"/>
+    <row r="176" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="36"/>
       <c r="B176" s="4" t="s">
         <v>142</v>
       </c>
@@ -7823,8 +7808,8 @@
       <c r="L176" s="4"/>
       <c r="M176" s="7"/>
     </row>
-    <row r="177" spans="1:13" ht="28" customHeight="1">
-      <c r="A177" s="38"/>
+    <row r="177" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A177" s="36"/>
       <c r="B177" s="4" t="s">
         <v>143</v>
       </c>
@@ -7856,8 +7841,8 @@
       <c r="L177" s="4"/>
       <c r="M177" s="7"/>
     </row>
-    <row r="178" spans="1:13" ht="28" customHeight="1">
-      <c r="A178" s="38"/>
+    <row r="178" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A178" s="36"/>
       <c r="B178" s="4" t="s">
         <v>144</v>
       </c>
@@ -7889,8 +7874,8 @@
       <c r="L178" s="4"/>
       <c r="M178" s="7"/>
     </row>
-    <row r="179" spans="1:13" ht="28" customHeight="1">
-      <c r="A179" s="38"/>
+    <row r="179" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A179" s="36"/>
       <c r="B179" s="4" t="s">
         <v>145</v>
       </c>
@@ -7922,8 +7907,8 @@
       <c r="L179" s="4"/>
       <c r="M179" s="7"/>
     </row>
-    <row r="180" spans="1:13" ht="28" customHeight="1">
-      <c r="A180" s="38"/>
+    <row r="180" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A180" s="36"/>
       <c r="B180" s="4" t="s">
         <v>146</v>
       </c>
@@ -7955,8 +7940,8 @@
       <c r="L180" s="4"/>
       <c r="M180" s="7"/>
     </row>
-    <row r="181" spans="1:13" ht="28" customHeight="1">
-      <c r="A181" s="38"/>
+    <row r="181" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="36"/>
       <c r="B181" s="4" t="s">
         <v>147</v>
       </c>
@@ -7988,8 +7973,8 @@
       <c r="L181" s="4"/>
       <c r="M181" s="7"/>
     </row>
-    <row r="182" spans="1:13" ht="28" customHeight="1">
-      <c r="A182" s="38"/>
+    <row r="182" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A182" s="36"/>
       <c r="B182" s="4" t="s">
         <v>145</v>
       </c>
@@ -8021,8 +8006,8 @@
       <c r="L182" s="4"/>
       <c r="M182" s="7"/>
     </row>
-    <row r="183" spans="1:13" ht="28" customHeight="1">
-      <c r="A183" s="38"/>
+    <row r="183" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A183" s="36"/>
       <c r="B183" s="4" t="s">
         <v>148</v>
       </c>
@@ -8054,8 +8039,8 @@
       <c r="L183" s="4"/>
       <c r="M183" s="7"/>
     </row>
-    <row r="184" spans="1:13" ht="28" customHeight="1">
-      <c r="A184" s="38"/>
+    <row r="184" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="36"/>
       <c r="B184" s="4" t="s">
         <v>149</v>
       </c>
@@ -8087,15 +8072,15 @@
       <c r="L184" s="4"/>
       <c r="M184" s="7"/>
     </row>
-    <row r="185" spans="1:13" ht="28" customHeight="1">
-      <c r="A185" s="38"/>
+    <row r="185" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="36"/>
       <c r="B185" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C185" s="4">
         <v>2012</v>
       </c>
-      <c r="D185" s="33">
+      <c r="D185" s="27">
         <v>23128226</v>
       </c>
       <c r="E185" s="5" t="s">
@@ -8126,15 +8111,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:13" ht="28" customHeight="1">
-      <c r="A186" s="38"/>
+    <row r="186" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A186" s="36"/>
       <c r="B186" s="17" t="s">
         <v>76</v>
       </c>
       <c r="C186" s="18">
         <v>2003</v>
       </c>
-      <c r="D186" s="33">
+      <c r="D186" s="27">
         <v>14685227</v>
       </c>
       <c r="E186" s="5" t="s">
@@ -8163,8 +8148,8 @@
       </c>
       <c r="M186" s="7"/>
     </row>
-    <row r="187" spans="1:13" ht="28" customHeight="1">
-      <c r="A187" s="38"/>
+    <row r="187" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A187" s="36"/>
       <c r="B187" s="4" t="s">
         <v>150</v>
       </c>
@@ -8196,8 +8181,8 @@
       <c r="L187" s="4"/>
       <c r="M187" s="7"/>
     </row>
-    <row r="188" spans="1:13" ht="28" customHeight="1">
-      <c r="A188" s="38"/>
+    <row r="188" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A188" s="36"/>
       <c r="B188" s="4" t="s">
         <v>151</v>
       </c>
@@ -8229,8 +8214,8 @@
       <c r="L188" s="4"/>
       <c r="M188" s="7"/>
     </row>
-    <row r="189" spans="1:13" ht="28" customHeight="1">
-      <c r="A189" s="38"/>
+    <row r="189" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="36"/>
       <c r="B189" s="4" t="s">
         <v>152</v>
       </c>
@@ -8266,8 +8251,8 @@
       </c>
       <c r="M189" s="7"/>
     </row>
-    <row r="190" spans="1:13" ht="28" customHeight="1">
-      <c r="A190" s="38"/>
+    <row r="190" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="36"/>
       <c r="B190" s="4" t="s">
         <v>152</v>
       </c>
@@ -8303,8 +8288,8 @@
       </c>
       <c r="M190" s="7"/>
     </row>
-    <row r="191" spans="1:13" ht="28" customHeight="1">
-      <c r="A191" s="38"/>
+    <row r="191" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A191" s="36"/>
       <c r="B191" s="4" t="s">
         <v>152</v>
       </c>
@@ -8340,8 +8325,8 @@
       </c>
       <c r="M191" s="7"/>
     </row>
-    <row r="192" spans="1:13" ht="28" customHeight="1">
-      <c r="A192" s="38"/>
+    <row r="192" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A192" s="36"/>
       <c r="B192" s="4" t="s">
         <v>152</v>
       </c>
@@ -8377,8 +8362,8 @@
       </c>
       <c r="M192" s="7"/>
     </row>
-    <row r="193" spans="1:13" ht="28" customHeight="1">
-      <c r="A193" s="38"/>
+    <row r="193" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="36"/>
       <c r="B193" s="17" t="s">
         <v>153</v>
       </c>
@@ -8412,8 +8397,8 @@
       </c>
       <c r="M193" s="7"/>
     </row>
-    <row r="194" spans="1:13" ht="28" customHeight="1">
-      <c r="A194" s="38"/>
+    <row r="194" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="36"/>
       <c r="B194" s="4" t="s">
         <v>154</v>
       </c>
@@ -8445,8 +8430,8 @@
       <c r="L194" s="4"/>
       <c r="M194" s="7"/>
     </row>
-    <row r="195" spans="1:13" ht="28" customHeight="1">
-      <c r="A195" s="38"/>
+    <row r="195" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A195" s="36"/>
       <c r="B195" s="4" t="s">
         <v>155</v>
       </c>
@@ -8478,8 +8463,8 @@
       <c r="L195" s="4"/>
       <c r="M195" s="7"/>
     </row>
-    <row r="196" spans="1:13" ht="28" customHeight="1">
-      <c r="A196" s="38"/>
+    <row r="196" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A196" s="36"/>
       <c r="B196" s="4" t="s">
         <v>156</v>
       </c>
@@ -8511,8 +8496,8 @@
       <c r="L196" s="4"/>
       <c r="M196" s="7"/>
     </row>
-    <row r="197" spans="1:13" ht="28" customHeight="1">
-      <c r="A197" s="38"/>
+    <row r="197" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="36"/>
       <c r="B197" s="4" t="s">
         <v>157</v>
       </c>
@@ -8544,8 +8529,8 @@
       <c r="L197" s="4"/>
       <c r="M197" s="7"/>
     </row>
-    <row r="198" spans="1:13" ht="28" customHeight="1">
-      <c r="A198" s="38"/>
+    <row r="198" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="36"/>
       <c r="B198" s="4" t="s">
         <v>158</v>
       </c>
@@ -8577,8 +8562,8 @@
       <c r="L198" s="4"/>
       <c r="M198" s="7"/>
     </row>
-    <row r="199" spans="1:13" ht="28" customHeight="1">
-      <c r="A199" s="38"/>
+    <row r="199" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A199" s="36"/>
       <c r="B199" s="4" t="s">
         <v>159</v>
       </c>
@@ -8610,8 +8595,8 @@
       <c r="L199" s="4"/>
       <c r="M199" s="7"/>
     </row>
-    <row r="200" spans="1:13" ht="28" customHeight="1">
-      <c r="A200" s="38"/>
+    <row r="200" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A200" s="36"/>
       <c r="B200" s="4" t="s">
         <v>160</v>
       </c>
@@ -8643,8 +8628,8 @@
       <c r="L200" s="4"/>
       <c r="M200" s="7"/>
     </row>
-    <row r="201" spans="1:13" ht="28" customHeight="1">
-      <c r="A201" s="38"/>
+    <row r="201" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A201" s="36"/>
       <c r="B201" s="4" t="s">
         <v>156</v>
       </c>
@@ -8676,8 +8661,8 @@
       <c r="L201" s="4"/>
       <c r="M201" s="7"/>
     </row>
-    <row r="202" spans="1:13" ht="28" customHeight="1">
-      <c r="A202" s="38"/>
+    <row r="202" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A202" s="36"/>
       <c r="B202" s="4" t="s">
         <v>158</v>
       </c>
@@ -8709,8 +8694,8 @@
       <c r="L202" s="4"/>
       <c r="M202" s="7"/>
     </row>
-    <row r="203" spans="1:13" ht="28" customHeight="1">
-      <c r="A203" s="38"/>
+    <row r="203" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="36"/>
       <c r="B203" s="4" t="s">
         <v>161</v>
       </c>
@@ -8742,8 +8727,8 @@
       <c r="L203" s="4"/>
       <c r="M203" s="7"/>
     </row>
-    <row r="204" spans="1:13" ht="28" customHeight="1">
-      <c r="A204" s="38"/>
+    <row r="204" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A204" s="36"/>
       <c r="B204" s="4" t="s">
         <v>80</v>
       </c>
@@ -8775,8 +8760,8 @@
       <c r="L204" s="4"/>
       <c r="M204" s="7"/>
     </row>
-    <row r="205" spans="1:13" ht="28" customHeight="1">
-      <c r="A205" s="34" t="s">
+    <row r="205" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A205" s="33" t="s">
         <v>274</v>
       </c>
       <c r="B205" s="23" t="s">
@@ -8802,8 +8787,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:13" ht="28" customHeight="1">
-      <c r="A206" s="35"/>
+    <row r="206" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="34"/>
       <c r="B206" s="19" t="s">
         <v>259</v>
       </c>
@@ -8827,8 +8812,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="207" spans="1:13" ht="28" customHeight="1">
-      <c r="A207" s="36"/>
+    <row r="207" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="35"/>
       <c r="B207" s="19" t="s">
         <v>261</v>
       </c>
@@ -8852,7 +8837,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="208" spans="1:13" ht="28" customHeight="1">
+    <row r="208" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A208" s="37"/>
       <c r="B208" s="4" t="s">
         <v>162</v>
@@ -8860,7 +8845,7 @@
       <c r="C208" s="4">
         <v>2011</v>
       </c>
-      <c r="D208" s="33">
+      <c r="D208" s="27">
         <v>21711429</v>
       </c>
       <c r="E208" s="5" t="s">
@@ -8885,8 +8870,8 @@
       <c r="L208" s="4"/>
       <c r="M208" s="7"/>
     </row>
-    <row r="209" spans="1:13" ht="28" customHeight="1">
-      <c r="A209" s="38"/>
+    <row r="209" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A209" s="36"/>
       <c r="B209" s="4" t="s">
         <v>163</v>
       </c>
@@ -8918,8 +8903,8 @@
       <c r="L209" s="4"/>
       <c r="M209" s="7"/>
     </row>
-    <row r="210" spans="1:13" ht="28" customHeight="1">
-      <c r="A210" s="38"/>
+    <row r="210" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A210" s="36"/>
       <c r="B210" s="4" t="s">
         <v>164</v>
       </c>
@@ -8955,15 +8940,15 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="211" spans="1:13" ht="28" customHeight="1">
-      <c r="A211" s="38"/>
+    <row r="211" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A211" s="36"/>
       <c r="B211" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C211" s="4">
         <v>2012</v>
       </c>
-      <c r="D211" s="33">
+      <c r="D211" s="27">
         <v>23128226</v>
       </c>
       <c r="E211" s="5" t="s">
@@ -8994,8 +8979,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:13" ht="28" customHeight="1">
-      <c r="A212" s="38"/>
+    <row r="212" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="36"/>
       <c r="B212" s="4" t="s">
         <v>155</v>
       </c>
@@ -9027,8 +9012,8 @@
       <c r="L212" s="4"/>
       <c r="M212" s="7"/>
     </row>
-    <row r="213" spans="1:13" ht="28" customHeight="1">
-      <c r="A213" s="38"/>
+    <row r="213" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="36"/>
       <c r="B213" s="4" t="s">
         <v>155</v>
       </c>
@@ -9060,8 +9045,8 @@
       <c r="L213" s="4"/>
       <c r="M213" s="7"/>
     </row>
-    <row r="214" spans="1:13" ht="28" customHeight="1">
-      <c r="A214" s="38"/>
+    <row r="214" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A214" s="36"/>
       <c r="B214" s="4" t="s">
         <v>165</v>
       </c>
@@ -9093,15 +9078,15 @@
       <c r="L214" s="4"/>
       <c r="M214" s="7"/>
     </row>
-    <row r="215" spans="1:13" ht="28" customHeight="1">
-      <c r="A215" s="38"/>
+    <row r="215" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A215" s="36"/>
       <c r="B215" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C215" s="4">
         <v>2012</v>
       </c>
-      <c r="D215" s="33">
+      <c r="D215" s="27">
         <v>23128226</v>
       </c>
       <c r="E215" s="5" t="s">
@@ -9132,15 +9117,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:13" ht="28" customHeight="1">
-      <c r="A216" s="38"/>
+    <row r="216" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="36"/>
       <c r="B216" s="17" t="s">
         <v>76</v>
       </c>
       <c r="C216" s="18">
         <v>2003</v>
       </c>
-      <c r="D216" s="33">
+      <c r="D216" s="27">
         <v>14685227</v>
       </c>
       <c r="E216" s="5" t="s">
@@ -9169,15 +9154,15 @@
       </c>
       <c r="M216" s="7"/>
     </row>
-    <row r="217" spans="1:13" ht="28" customHeight="1">
-      <c r="A217" s="38"/>
+    <row r="217" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="36"/>
       <c r="B217" s="4" t="s">
         <v>155</v>
       </c>
       <c r="C217" s="4">
         <v>2007</v>
       </c>
-      <c r="D217" s="33">
+      <c r="D217" s="27">
         <v>17667794</v>
       </c>
       <c r="E217" s="5" t="s">
@@ -9202,15 +9187,15 @@
       <c r="L217" s="4"/>
       <c r="M217" s="7"/>
     </row>
-    <row r="218" spans="1:13" ht="28" customHeight="1">
-      <c r="A218" s="38"/>
+    <row r="218" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="36"/>
       <c r="B218" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C218" s="4">
         <v>2012</v>
       </c>
-      <c r="D218" s="33">
+      <c r="D218" s="27">
         <v>23128226</v>
       </c>
       <c r="E218" s="5" t="s">
@@ -9239,8 +9224,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:13" ht="28" customHeight="1">
-      <c r="A219" s="34" t="s">
+    <row r="219" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="33" t="s">
         <v>275</v>
       </c>
       <c r="B219" s="23" t="s">
@@ -9266,8 +9251,8 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="220" spans="1:13" ht="28" customHeight="1">
-      <c r="A220" s="35"/>
+    <row r="220" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="34"/>
       <c r="B220" s="19" t="s">
         <v>259</v>
       </c>
@@ -9291,8 +9276,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:13" ht="28" customHeight="1">
-      <c r="A221" s="36"/>
+    <row r="221" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="35"/>
       <c r="B221" s="19" t="s">
         <v>261</v>
       </c>
@@ -9316,7 +9301,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="222" spans="1:13" ht="28" customHeight="1">
+    <row r="222" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="37"/>
       <c r="B222" s="4" t="s">
         <v>79</v>
@@ -9355,8 +9340,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:13" ht="28" customHeight="1">
-      <c r="A223" s="38"/>
+    <row r="223" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A223" s="36"/>
       <c r="B223" s="4" t="s">
         <v>166</v>
       </c>
@@ -9388,8 +9373,8 @@
       <c r="L223" s="4"/>
       <c r="M223" s="7"/>
     </row>
-    <row r="224" spans="1:13" ht="28" customHeight="1">
-      <c r="A224" s="38"/>
+    <row r="224" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A224" s="36"/>
       <c r="B224" s="4" t="s">
         <v>167</v>
       </c>
@@ -9421,8 +9406,8 @@
       <c r="L224" s="4"/>
       <c r="M224" s="7"/>
     </row>
-    <row r="225" spans="1:13" ht="28" customHeight="1">
-      <c r="A225" s="38"/>
+    <row r="225" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A225" s="36"/>
       <c r="B225" s="4" t="s">
         <v>168</v>
       </c>
@@ -9454,8 +9439,8 @@
       <c r="L225" s="4"/>
       <c r="M225" s="7"/>
     </row>
-    <row r="226" spans="1:13" ht="28" customHeight="1">
-      <c r="A226" s="38"/>
+    <row r="226" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="36"/>
       <c r="B226" s="4" t="s">
         <v>169</v>
       </c>
@@ -9491,8 +9476,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:13" ht="28" customHeight="1">
-      <c r="A227" s="38"/>
+    <row r="227" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="36"/>
       <c r="B227" s="4" t="s">
         <v>170</v>
       </c>
@@ -9524,8 +9509,8 @@
       <c r="L227" s="4"/>
       <c r="M227" s="7"/>
     </row>
-    <row r="228" spans="1:13" ht="28" customHeight="1">
-      <c r="A228" s="38"/>
+    <row r="228" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A228" s="36"/>
       <c r="B228" s="4" t="s">
         <v>171</v>
       </c>
@@ -9557,8 +9542,8 @@
       <c r="L228" s="4"/>
       <c r="M228" s="7"/>
     </row>
-    <row r="229" spans="1:13" ht="28" customHeight="1">
-      <c r="A229" s="38"/>
+    <row r="229" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A229" s="36"/>
       <c r="B229" s="4" t="s">
         <v>79</v>
       </c>
@@ -9596,8 +9581,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:13" ht="28" customHeight="1">
-      <c r="A230" s="38"/>
+    <row r="230" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="36"/>
       <c r="B230" s="4" t="s">
         <v>79</v>
       </c>
@@ -9635,8 +9620,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="231" spans="1:13" ht="28" customHeight="1">
-      <c r="A231" s="38"/>
+    <row r="231" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="36"/>
       <c r="B231" s="4" t="s">
         <v>79</v>
       </c>
@@ -9674,8 +9659,8 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="232" spans="1:13" ht="28" customHeight="1">
-      <c r="A232" s="34" t="s">
+    <row r="232" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A232" s="33" t="s">
         <v>276</v>
       </c>
       <c r="B232" s="23" t="s">
@@ -9701,8 +9686,8 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="233" spans="1:13" ht="28" customHeight="1">
-      <c r="A233" s="35"/>
+    <row r="233" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A233" s="34"/>
       <c r="B233" s="19" t="s">
         <v>259</v>
       </c>
@@ -9726,8 +9711,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:13" ht="28" customHeight="1">
-      <c r="A234" s="36"/>
+    <row r="234" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="35"/>
       <c r="B234" s="19" t="s">
         <v>261</v>
       </c>
@@ -9751,7 +9736,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="235" spans="1:13" ht="28" customHeight="1">
+    <row r="235" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A235" s="37"/>
       <c r="B235" s="4" t="s">
         <v>172</v>
@@ -9784,8 +9769,8 @@
       <c r="L235" s="4"/>
       <c r="M235" s="7"/>
     </row>
-    <row r="236" spans="1:13" ht="28" customHeight="1">
-      <c r="A236" s="38"/>
+    <row r="236" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A236" s="36"/>
       <c r="B236" s="4" t="s">
         <v>173</v>
       </c>
@@ -9819,8 +9804,8 @@
       </c>
       <c r="M236" s="7"/>
     </row>
-    <row r="237" spans="1:13" ht="28" customHeight="1">
-      <c r="A237" s="38"/>
+    <row r="237" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A237" s="36"/>
       <c r="B237" s="4" t="s">
         <v>90</v>
       </c>
@@ -9854,8 +9839,8 @@
       </c>
       <c r="M237" s="7"/>
     </row>
-    <row r="238" spans="1:13" ht="28" customHeight="1">
-      <c r="A238" s="38"/>
+    <row r="238" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A238" s="36"/>
       <c r="B238" s="4" t="s">
         <v>174</v>
       </c>
@@ -9889,15 +9874,15 @@
       </c>
       <c r="M238" s="7"/>
     </row>
-    <row r="239" spans="1:13" ht="28" customHeight="1">
-      <c r="A239" s="38"/>
+    <row r="239" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A239" s="36"/>
       <c r="B239" s="17" t="s">
         <v>76</v>
       </c>
       <c r="C239" s="18">
         <v>2003</v>
       </c>
-      <c r="D239" s="33">
+      <c r="D239" s="27">
         <v>14685227</v>
       </c>
       <c r="E239" s="5" t="s">
@@ -9924,8 +9909,8 @@
       <c r="L239" s="4"/>
       <c r="M239" s="7"/>
     </row>
-    <row r="240" spans="1:13" ht="28" customHeight="1">
-      <c r="A240" s="38"/>
+    <row r="240" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="36"/>
       <c r="B240" s="4" t="s">
         <v>175</v>
       </c>
@@ -9957,8 +9942,8 @@
       <c r="L240" s="4"/>
       <c r="M240" s="7"/>
     </row>
-    <row r="241" spans="1:13" ht="28" customHeight="1">
-      <c r="A241" s="38"/>
+    <row r="241" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A241" s="36"/>
       <c r="B241" s="8" t="s">
         <v>176</v>
       </c>
@@ -9994,8 +9979,8 @@
       </c>
       <c r="M241" s="14"/>
     </row>
-    <row r="242" spans="1:13" ht="28" customHeight="1">
-      <c r="A242" s="34" t="s">
+    <row r="242" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A242" s="33" t="s">
         <v>277</v>
       </c>
       <c r="B242" s="23" t="s">
@@ -10021,8 +10006,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="243" spans="1:13" ht="28" customHeight="1">
-      <c r="A243" s="35"/>
+    <row r="243" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="34"/>
       <c r="B243" s="19" t="s">
         <v>259</v>
       </c>
@@ -10046,8 +10031,8 @@
         <v>262</v>
       </c>
     </row>
-    <row r="244" spans="1:13" ht="28" customHeight="1">
-      <c r="A244" s="36"/>
+    <row r="244" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="35"/>
       <c r="B244" s="19" t="s">
         <v>261</v>
       </c>
@@ -10071,24 +10056,32 @@
         <v>262</v>
       </c>
     </row>
-    <row r="245" spans="1:13" ht="28" customHeight="1">
-      <c r="B245" s="39" t="s">
+    <row r="245" spans="1:13" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B245" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="C245" s="39"/>
-      <c r="D245" s="39"/>
-      <c r="E245" s="39"/>
-      <c r="F245" s="39"/>
-      <c r="G245" s="39"/>
-      <c r="H245" s="39"/>
-      <c r="I245" s="39"/>
-      <c r="J245" s="39"/>
-      <c r="K245" s="39"/>
-      <c r="L245" s="39"/>
-      <c r="M245" s="39"/>
+      <c r="C245" s="32"/>
+      <c r="D245" s="32"/>
+      <c r="E245" s="32"/>
+      <c r="F245" s="32"/>
+      <c r="G245" s="32"/>
+      <c r="H245" s="32"/>
+      <c r="I245" s="32"/>
+      <c r="J245" s="32"/>
+      <c r="K245" s="32"/>
+      <c r="L245" s="32"/>
+      <c r="M245" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="A232:A234"/>
+    <mergeCell ref="A235:A241"/>
+    <mergeCell ref="A242:A244"/>
+    <mergeCell ref="A157:A204"/>
+    <mergeCell ref="A205:A207"/>
+    <mergeCell ref="A208:A218"/>
+    <mergeCell ref="A219:A221"/>
+    <mergeCell ref="A222:A231"/>
     <mergeCell ref="B245:M245"/>
     <mergeCell ref="A10:A12"/>
     <mergeCell ref="A1:A9"/>
@@ -10105,1716 +10098,8 @@
     <mergeCell ref="A75:A77"/>
     <mergeCell ref="A78:A153"/>
     <mergeCell ref="A154:A156"/>
-    <mergeCell ref="A232:A234"/>
-    <mergeCell ref="A235:A241"/>
-    <mergeCell ref="A242:A244"/>
-    <mergeCell ref="A157:A204"/>
-    <mergeCell ref="A205:A207"/>
-    <mergeCell ref="A208:A218"/>
-    <mergeCell ref="A219:A221"/>
-    <mergeCell ref="A222:A231"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U74"/>
-  <sheetViews>
-    <sheetView topLeftCell="G48" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:21">
-      <c r="A1" s="5"/>
-      <c r="B1" s="7"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6"/>
-    </row>
-    <row r="2" spans="1:21">
-      <c r="A2" s="5"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
-    </row>
-    <row r="3" spans="1:21">
-      <c r="A3" s="5"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
-    </row>
-    <row r="4" spans="1:21">
-      <c r="A4" s="5"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="17"/>
-      <c r="K4" s="27"/>
-      <c r="M4" s="16"/>
-      <c r="O4" s="27"/>
-      <c r="Q4" s="6">
-        <v>23</v>
-      </c>
-      <c r="R4" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="S4">
-        <f>Q4*R4</f>
-        <v>2.99</v>
-      </c>
-      <c r="T4" s="7">
-        <v>0.87</v>
-      </c>
-      <c r="U4">
-        <f>T4*Q4</f>
-        <v>20.010000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="5"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="28"/>
-      <c r="K5" s="29"/>
-      <c r="M5" s="32"/>
-      <c r="O5" s="29"/>
-      <c r="Q5" s="6">
-        <v>20</v>
-      </c>
-      <c r="R5" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="S5">
-        <f>R5*Q5</f>
-        <v>5</v>
-      </c>
-      <c r="T5" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="U5">
-        <f>T5*Q5</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21">
-      <c r="A6" s="5"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="28"/>
-      <c r="K6" s="29"/>
-      <c r="M6" s="30"/>
-      <c r="O6" s="31"/>
-      <c r="Q6" s="6">
-        <v>85</v>
-      </c>
-      <c r="R6" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="S6">
-        <f t="shared" ref="S6:S52" si="0">Q6*R6</f>
-        <v>4.25</v>
-      </c>
-      <c r="T6" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="U6">
-        <f t="shared" ref="U6:U52" si="1">T6*Q6</f>
-        <v>80.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21">
-      <c r="A7" s="5"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="28"/>
-      <c r="K7" s="29"/>
-      <c r="M7" s="30"/>
-      <c r="O7" s="31"/>
-      <c r="Q7" s="6">
-        <v>111</v>
-      </c>
-      <c r="R7" s="5">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="S7">
-        <f t="shared" si="0"/>
-        <v>3.9959999999999996</v>
-      </c>
-      <c r="T7" s="7">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="U7">
-        <f t="shared" si="1"/>
-        <v>107.00399999999999</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21">
-      <c r="A8" s="5"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="28"/>
-      <c r="K8" s="29"/>
-      <c r="M8" s="30"/>
-      <c r="O8" s="31"/>
-      <c r="Q8" s="6">
-        <v>166</v>
-      </c>
-      <c r="R8" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="S8">
-        <f t="shared" si="0"/>
-        <v>13.280000000000001</v>
-      </c>
-      <c r="T8" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="U8">
-        <f t="shared" si="1"/>
-        <v>152.72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21">
-      <c r="A9" s="5"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="7"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="28"/>
-      <c r="K9" s="29"/>
-      <c r="M9" s="30"/>
-      <c r="O9" s="31"/>
-      <c r="Q9" s="6">
-        <v>15</v>
-      </c>
-      <c r="R9" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S9">
-        <f t="shared" si="0"/>
-        <v>1.05</v>
-      </c>
-      <c r="T9" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="U9">
-        <f t="shared" si="1"/>
-        <v>13.950000000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21">
-      <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="7"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="28"/>
-      <c r="K10" s="29"/>
-      <c r="M10" s="30"/>
-      <c r="O10" s="31"/>
-      <c r="Q10" s="6">
-        <v>59</v>
-      </c>
-      <c r="R10" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="0"/>
-        <v>4.72</v>
-      </c>
-      <c r="T10" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="U10">
-        <f t="shared" si="1"/>
-        <v>54.28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21">
-      <c r="A11" s="5"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="7"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="28"/>
-      <c r="K11" s="29"/>
-      <c r="M11" s="30"/>
-      <c r="O11" s="31"/>
-      <c r="Q11" s="6">
-        <v>50</v>
-      </c>
-      <c r="R11" s="5">
-        <v>0.13</v>
-      </c>
-      <c r="S11">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="T11" s="7">
-        <v>0.87</v>
-      </c>
-      <c r="U11">
-        <f t="shared" si="1"/>
-        <v>43.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21">
-      <c r="A12" s="5"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="7"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="28"/>
-      <c r="K12" s="29"/>
-      <c r="M12" s="30"/>
-      <c r="O12" s="29"/>
-      <c r="Q12" s="6">
-        <v>140</v>
-      </c>
-      <c r="R12" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S12">
-        <f t="shared" si="0"/>
-        <v>9.8000000000000007</v>
-      </c>
-      <c r="T12" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="U12">
-        <f t="shared" si="1"/>
-        <v>130.20000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21">
-      <c r="A13" s="5"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="7"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="28"/>
-      <c r="K13" s="29"/>
-      <c r="M13" s="30"/>
-      <c r="O13" s="29"/>
-      <c r="Q13" s="6">
-        <v>89</v>
-      </c>
-      <c r="R13" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="S13">
-        <f t="shared" si="0"/>
-        <v>5.34</v>
-      </c>
-      <c r="T13" s="7">
-        <v>0.94</v>
-      </c>
-      <c r="U13">
-        <f t="shared" si="1"/>
-        <v>83.66</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21">
-      <c r="A14" s="5"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="7"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="M14" s="30"/>
-      <c r="O14" s="31"/>
-      <c r="Q14" s="6">
-        <v>160</v>
-      </c>
-      <c r="R14" s="5">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="S14">
-        <f t="shared" si="0"/>
-        <v>11.040000000000001</v>
-      </c>
-      <c r="T14" s="7">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="U14">
-        <f t="shared" si="1"/>
-        <v>148.96</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="7"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="28"/>
-      <c r="K15" s="29"/>
-      <c r="M15" s="32"/>
-      <c r="O15" s="29"/>
-      <c r="Q15" s="6">
-        <v>77</v>
-      </c>
-      <c r="R15" s="5">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="S15">
-        <f t="shared" si="0"/>
-        <v>5.4669999999999996</v>
-      </c>
-      <c r="T15" s="7">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="U15">
-        <f t="shared" si="1"/>
-        <v>71.533000000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21">
-      <c r="A16" s="5"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="7"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="28"/>
-      <c r="K16" s="29"/>
-      <c r="M16" s="30"/>
-      <c r="O16" s="31"/>
-      <c r="Q16" s="6">
-        <v>500</v>
-      </c>
-      <c r="R16" s="5">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S16">
-        <f t="shared" si="0"/>
-        <v>41</v>
-      </c>
-      <c r="T16" s="7">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="U16">
-        <f t="shared" si="1"/>
-        <v>458.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:21">
-      <c r="A17" s="5"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="7"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="28"/>
-      <c r="K17" s="29"/>
-      <c r="M17" s="30"/>
-      <c r="O17" s="31"/>
-      <c r="Q17" s="6">
-        <v>49</v>
-      </c>
-      <c r="R17" s="5">
-        <v>0.16</v>
-      </c>
-      <c r="S17">
-        <f t="shared" si="0"/>
-        <v>7.84</v>
-      </c>
-      <c r="T17" s="7">
-        <v>0.84</v>
-      </c>
-      <c r="U17">
-        <f t="shared" si="1"/>
-        <v>41.16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:21">
-      <c r="A18" s="5"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="7"/>
-      <c r="Q18" s="6">
-        <v>27</v>
-      </c>
-      <c r="R18" s="5">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="S18">
-        <f t="shared" si="0"/>
-        <v>3.996</v>
-      </c>
-      <c r="T18" s="7">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="U18">
-        <f t="shared" si="1"/>
-        <v>23.003999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="1:21">
-      <c r="A19" s="5"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="7"/>
-      <c r="Q19" s="6">
-        <v>449</v>
-      </c>
-      <c r="R19" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="S19">
-        <f t="shared" si="0"/>
-        <v>35.92</v>
-      </c>
-      <c r="T19" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="U19">
-        <f t="shared" si="1"/>
-        <v>413.08000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:21">
-      <c r="A20" s="5"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="7"/>
-      <c r="Q20" s="6">
-        <v>93</v>
-      </c>
-      <c r="R20" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="S20">
-        <f t="shared" si="0"/>
-        <v>4.6500000000000004</v>
-      </c>
-      <c r="T20" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="U20">
-        <f t="shared" si="1"/>
-        <v>88.35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:21">
-      <c r="A21" s="5"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="7"/>
-      <c r="Q21" s="6">
-        <v>51</v>
-      </c>
-      <c r="R21" s="5">
-        <v>0.187</v>
-      </c>
-      <c r="S21">
-        <f t="shared" si="0"/>
-        <v>9.5370000000000008</v>
-      </c>
-      <c r="T21" s="7">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="U21">
-        <f t="shared" si="1"/>
-        <v>41.462999999999994</v>
-      </c>
-    </row>
-    <row r="22" spans="1:21">
-      <c r="A22" s="5"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="7"/>
-      <c r="Q22" s="6">
-        <v>50</v>
-      </c>
-      <c r="R22" s="5">
-        <v>0.11</v>
-      </c>
-      <c r="S22">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
-      <c r="T22" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="U22">
-        <f t="shared" si="1"/>
-        <v>44.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:21">
-      <c r="A23" s="5"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="7"/>
-      <c r="Q23" s="6">
-        <v>40</v>
-      </c>
-      <c r="R23" s="5">
-        <v>0.16300000000000001</v>
-      </c>
-      <c r="S23">
-        <f t="shared" si="0"/>
-        <v>6.5200000000000005</v>
-      </c>
-      <c r="T23" s="7">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="U23">
-        <f t="shared" si="1"/>
-        <v>33.479999999999997</v>
-      </c>
-    </row>
-    <row r="24" spans="1:21">
-      <c r="A24" s="5"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="7"/>
-      <c r="Q24" s="6">
-        <v>74</v>
-      </c>
-      <c r="R24" s="5">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="S24">
-        <f t="shared" si="0"/>
-        <v>4.9580000000000002</v>
-      </c>
-      <c r="T24" s="7">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="U24">
-        <f t="shared" si="1"/>
-        <v>69.042000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:21">
-      <c r="A25" s="5"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="7"/>
-      <c r="Q25" s="6">
-        <v>134</v>
-      </c>
-      <c r="R25" s="5">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="S25">
-        <f t="shared" si="0"/>
-        <v>10.854000000000001</v>
-      </c>
-      <c r="T25" s="7">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="U25">
-        <f t="shared" si="1"/>
-        <v>123.146</v>
-      </c>
-    </row>
-    <row r="26" spans="1:21">
-      <c r="A26" s="5"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="7"/>
-      <c r="J26" s="7">
-        <v>0.75</v>
-      </c>
-      <c r="L26" s="5">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="Q26" s="6">
-        <v>283</v>
-      </c>
-      <c r="R26" s="5">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="S26">
-        <f t="shared" si="0"/>
-        <v>15.848000000000001</v>
-      </c>
-      <c r="T26" s="7">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="U26">
-        <f t="shared" si="1"/>
-        <v>267.15199999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:21">
-      <c r="A27" s="5"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="7"/>
-      <c r="J27" s="7">
-        <v>0.81299999999999994</v>
-      </c>
-      <c r="L27" s="5">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="Q27" s="6">
-        <v>51</v>
-      </c>
-      <c r="R27" s="5">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="S27">
-        <f t="shared" si="0"/>
-        <v>4.2330000000000005</v>
-      </c>
-      <c r="T27" s="7">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="U27">
-        <f t="shared" si="1"/>
-        <v>46.767000000000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:21">
-      <c r="A28" s="5"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="7"/>
-      <c r="J28" s="7">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="L28" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="Q28" s="6">
-        <v>143</v>
-      </c>
-      <c r="R28" s="5">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="S28">
-        <f t="shared" si="0"/>
-        <v>8.0080000000000009</v>
-      </c>
-      <c r="T28" s="7">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="U28">
-        <f t="shared" si="1"/>
-        <v>134.99199999999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:21">
-      <c r="A29" s="5"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="7"/>
-      <c r="J29" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="L29" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="Q29" s="6">
-        <v>26</v>
-      </c>
-      <c r="R29" s="5">
-        <v>0.12</v>
-      </c>
-      <c r="S29">
-        <f t="shared" si="0"/>
-        <v>3.12</v>
-      </c>
-      <c r="T29" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="U29">
-        <f t="shared" si="1"/>
-        <v>22.88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:21">
-      <c r="A30" s="5"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="7"/>
-      <c r="J30" s="7">
-        <v>0.83699999999999997</v>
-      </c>
-      <c r="L30" s="5">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="Q30" s="6">
-        <v>32</v>
-      </c>
-      <c r="R30" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S30">
-        <f t="shared" si="0"/>
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="T30" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="U30">
-        <f t="shared" si="1"/>
-        <v>29.76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21">
-      <c r="A31" s="5"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="7"/>
-      <c r="J31" s="7">
-        <v>0.84</v>
-      </c>
-      <c r="L31" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="Q31" s="6">
-        <v>92</v>
-      </c>
-      <c r="R31" s="5">
-        <v>0.115</v>
-      </c>
-      <c r="S31">
-        <f t="shared" si="0"/>
-        <v>10.58</v>
-      </c>
-      <c r="T31" s="7">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="U31">
-        <f t="shared" si="1"/>
-        <v>81.42</v>
-      </c>
-    </row>
-    <row r="32" spans="1:21">
-      <c r="A32" s="5"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="7"/>
-      <c r="J32" s="7">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="L32" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="Q32" s="6">
-        <v>27</v>
-      </c>
-      <c r="R32" s="5">
-        <v>0.17</v>
-      </c>
-      <c r="S32">
-        <f t="shared" si="0"/>
-        <v>4.5900000000000007</v>
-      </c>
-      <c r="T32" s="7">
-        <v>0.83</v>
-      </c>
-      <c r="U32">
-        <f t="shared" si="1"/>
-        <v>22.41</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21">
-      <c r="A33" s="5"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="7"/>
-      <c r="J33" s="7">
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="L33" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="Q33" s="6">
-        <v>98</v>
-      </c>
-      <c r="R33" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="S33">
-        <f t="shared" si="0"/>
-        <v>3.92</v>
-      </c>
-      <c r="T33" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="U33">
-        <f t="shared" si="1"/>
-        <v>93.1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21">
-      <c r="A34" s="5"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="4"/>
-      <c r="D34" s="7"/>
-      <c r="J34" s="7">
-        <v>0.87</v>
-      </c>
-      <c r="L34" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="Q34" s="6">
-        <v>102</v>
-      </c>
-      <c r="R34" s="5">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="S34">
-        <f t="shared" si="0"/>
-        <v>4.9980000000000002</v>
-      </c>
-      <c r="T34" s="7">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="U34">
-        <f t="shared" si="1"/>
-        <v>96.49199999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21">
-      <c r="A35" s="5"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="7"/>
-      <c r="J35" s="7">
-        <v>0.87</v>
-      </c>
-      <c r="L35" s="5">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="Q35" s="6">
-        <v>200</v>
-      </c>
-      <c r="R35" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="S35">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="T35" s="7">
-        <v>0.94</v>
-      </c>
-      <c r="U35">
-        <f t="shared" si="1"/>
-        <v>188</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21">
-      <c r="A36" s="5"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="7"/>
-      <c r="J36" s="7">
-        <v>0.88</v>
-      </c>
-      <c r="L36" s="5">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="Q36" s="6">
-        <v>241</v>
-      </c>
-      <c r="R36" s="5">
-        <v>3.6999999999999998E-2</v>
-      </c>
-      <c r="S36">
-        <f t="shared" si="0"/>
-        <v>8.9169999999999998</v>
-      </c>
-      <c r="T36" s="7">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="U36">
-        <f t="shared" si="1"/>
-        <v>232.083</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21">
-      <c r="A37" s="5"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="7"/>
-      <c r="J37" s="7">
-        <v>0.88500000000000001</v>
-      </c>
-      <c r="L37" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="Q37" s="6">
-        <v>87</v>
-      </c>
-      <c r="R37" s="5">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="S37">
-        <f t="shared" si="0"/>
-        <v>12.527999999999999</v>
-      </c>
-      <c r="T37" s="7">
-        <v>0.85599999999999998</v>
-      </c>
-      <c r="U37">
-        <f t="shared" si="1"/>
-        <v>74.471999999999994</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21">
-      <c r="A38" s="5"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="4"/>
-      <c r="D38" s="7"/>
-      <c r="J38" s="7">
-        <v>0.89</v>
-      </c>
-      <c r="L38" s="5">
-        <v>0.06</v>
-      </c>
-      <c r="Q38" s="6">
-        <v>87</v>
-      </c>
-      <c r="R38" s="5">
-        <v>0.17799999999999999</v>
-      </c>
-      <c r="S38">
-        <f t="shared" si="0"/>
-        <v>15.485999999999999</v>
-      </c>
-      <c r="T38" s="7">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="U38">
-        <f t="shared" si="1"/>
-        <v>71.513999999999996</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21">
-      <c r="A39" s="5"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="7"/>
-      <c r="J39" s="7">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="L39" s="5">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>85</v>
-      </c>
-      <c r="R39" s="5">
-        <v>0.106</v>
-      </c>
-      <c r="S39">
-        <f t="shared" si="0"/>
-        <v>9.01</v>
-      </c>
-      <c r="T39" s="7">
-        <v>0.89400000000000002</v>
-      </c>
-      <c r="U39">
-        <f t="shared" si="1"/>
-        <v>75.989999999999995</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21">
-      <c r="A40" s="5"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="7"/>
-      <c r="J40" s="7">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="L40" s="5">
-        <v>6.7000000000000004E-2</v>
-      </c>
-      <c r="Q40" s="6">
-        <v>88</v>
-      </c>
-      <c r="R40" s="5">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="S40">
-        <f t="shared" si="0"/>
-        <v>6.5119999999999996</v>
-      </c>
-      <c r="T40" s="7">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="U40">
-        <f t="shared" si="1"/>
-        <v>81.488</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21">
-      <c r="A41" s="5"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="4"/>
-      <c r="D41" s="7"/>
-      <c r="J41" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="L41" s="5">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="Q41" s="6">
-        <v>83</v>
-      </c>
-      <c r="R41" s="5">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="S41">
-        <f t="shared" si="0"/>
-        <v>6.9720000000000004</v>
-      </c>
-      <c r="T41" s="7">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="U41">
-        <f t="shared" si="1"/>
-        <v>76.028000000000006</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21">
-      <c r="A42" s="5"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="7"/>
-      <c r="J42" s="7">
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="L42" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q42" s="6">
-        <v>207</v>
-      </c>
-      <c r="R42" s="5">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="S42">
-        <f t="shared" si="0"/>
-        <v>13.455</v>
-      </c>
-      <c r="T42" s="7">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="U42">
-        <f t="shared" si="1"/>
-        <v>193.54500000000002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:21">
-      <c r="A43" s="5"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="7"/>
-      <c r="J43" s="7">
-        <v>0.91600000000000004</v>
-      </c>
-      <c r="L43" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>204</v>
-      </c>
-      <c r="R43" s="5">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="S43">
-        <f t="shared" si="0"/>
-        <v>17.543999999999997</v>
-      </c>
-      <c r="T43" s="7">
-        <v>0.91400000000000003</v>
-      </c>
-      <c r="U43">
-        <f t="shared" si="1"/>
-        <v>186.45600000000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21">
-      <c r="A44" s="5"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="4"/>
-      <c r="D44" s="7"/>
-      <c r="J44" s="7">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="L44" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q44" s="6">
-        <v>177</v>
-      </c>
-      <c r="R44" s="5">
-        <v>0.09</v>
-      </c>
-      <c r="S44">
-        <f t="shared" si="0"/>
-        <v>15.93</v>
-      </c>
-      <c r="T44" s="7">
-        <v>0.91</v>
-      </c>
-      <c r="U44">
-        <f t="shared" si="1"/>
-        <v>161.07</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21">
-      <c r="A45" s="5"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="4"/>
-      <c r="D45" s="7"/>
-      <c r="J45" s="7">
-        <v>0.91700000000000004</v>
-      </c>
-      <c r="L45" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="Q45" s="6">
-        <v>186</v>
-      </c>
-      <c r="R45" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="S45">
-        <f t="shared" si="0"/>
-        <v>14.88</v>
-      </c>
-      <c r="T45" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="U45">
-        <f t="shared" si="1"/>
-        <v>171.12</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="A46" s="5"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="7"/>
-      <c r="J46" s="7">
-        <v>0.91900000000000004</v>
-      </c>
-      <c r="L46" s="5">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>206</v>
-      </c>
-      <c r="R46" s="5">
-        <v>0.04</v>
-      </c>
-      <c r="S46">
-        <f t="shared" si="0"/>
-        <v>8.24</v>
-      </c>
-      <c r="T46" s="7">
-        <v>0.96</v>
-      </c>
-      <c r="U46">
-        <f t="shared" si="1"/>
-        <v>197.76</v>
-      </c>
-    </row>
-    <row r="47" spans="1:21">
-      <c r="A47" s="5"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="7"/>
-      <c r="J47" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="L47" s="5">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="Q47" s="6">
-        <v>50</v>
-      </c>
-      <c r="R47" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="S47">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="T47" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="U47">
-        <f t="shared" si="1"/>
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:21">
-      <c r="A48" s="5"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="7"/>
-      <c r="J48" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="L48" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="Q48" s="6">
-        <v>65</v>
-      </c>
-      <c r="R48" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="S48">
-        <f t="shared" si="0"/>
-        <v>5.2</v>
-      </c>
-      <c r="T48" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="U48">
-        <f t="shared" si="1"/>
-        <v>59.800000000000004</v>
-      </c>
-    </row>
-    <row r="49" spans="1:21">
-      <c r="A49" s="5"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="7"/>
-      <c r="J49" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="L49" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="Q49" s="6">
-        <v>103</v>
-      </c>
-      <c r="R49" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="S49">
-        <f t="shared" si="0"/>
-        <v>5.15</v>
-      </c>
-      <c r="T49" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="U49">
-        <f t="shared" si="1"/>
-        <v>97.85</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21">
-      <c r="A50" s="5"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="7"/>
-      <c r="J50" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="L50" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="Q50" s="6">
-        <v>400</v>
-      </c>
-      <c r="R50" s="5">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="S50">
-        <f t="shared" si="0"/>
-        <v>40.799999999999997</v>
-      </c>
-      <c r="T50" s="7">
-        <v>0.89800000000000002</v>
-      </c>
-      <c r="U50">
-        <f t="shared" si="1"/>
-        <v>359.2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:21">
-      <c r="A51" s="5"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="7"/>
-      <c r="J51" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="L51" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="Q51" s="6">
-        <v>53</v>
-      </c>
-      <c r="R51" s="5">
-        <v>0.05</v>
-      </c>
-      <c r="S51">
-        <f t="shared" si="0"/>
-        <v>2.6500000000000004</v>
-      </c>
-      <c r="T51" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="U51">
-        <f t="shared" si="1"/>
-        <v>50.349999999999994</v>
-      </c>
-    </row>
-    <row r="52" spans="1:21">
-      <c r="A52" s="5"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="7"/>
-      <c r="J52" s="7">
-        <v>0.92</v>
-      </c>
-      <c r="L52" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="Q52" s="6">
-        <v>136</v>
-      </c>
-      <c r="R52" s="5">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="S52">
-        <f t="shared" si="0"/>
-        <v>9.5200000000000014</v>
-      </c>
-      <c r="T52" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="U52">
-        <f t="shared" si="1"/>
-        <v>126.48</v>
-      </c>
-    </row>
-    <row r="53" spans="1:21">
-      <c r="A53" s="5"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="7"/>
-      <c r="J53" s="7">
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="L53" s="5">
-        <v>0.08</v>
-      </c>
-      <c r="Q53" s="24">
-        <f>SUM(Q4:Q52)</f>
-        <v>5974</v>
-      </c>
-      <c r="R53" s="24">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="S53">
-        <f>SUM(S4:S52)</f>
-        <v>470.53899999999999</v>
-      </c>
-      <c r="T53" s="23">
-        <v>0.92100000000000004</v>
-      </c>
-      <c r="U53">
-        <f>SUM(U4:U52)</f>
-        <v>5501.4710000000005</v>
-      </c>
-    </row>
-    <row r="54" spans="1:21">
-      <c r="A54" s="5"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="7"/>
-      <c r="J54" s="7">
-        <v>0.92900000000000005</v>
-      </c>
-      <c r="L54" s="5">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="S54">
-        <f>S53/Q53</f>
-        <v>7.8764479410780047E-2</v>
-      </c>
-      <c r="U54">
-        <f>U53/Q53</f>
-        <v>0.92090241044526289</v>
-      </c>
-    </row>
-    <row r="55" spans="1:21">
-      <c r="A55" s="5"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="7"/>
-      <c r="J55" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="L55" s="5">
-        <v>8.2000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="56" spans="1:21">
-      <c r="A56" s="5"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="7"/>
-      <c r="J56" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="L56" s="5">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="Q56">
-        <v>5954</v>
-      </c>
-      <c r="S56">
-        <v>7.8E-2</v>
-      </c>
-      <c r="U56">
-        <v>0.92100000000000004</v>
-      </c>
-    </row>
-    <row r="57" spans="1:21">
-      <c r="A57" s="5"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="7"/>
-      <c r="J57" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="L57" s="5">
-        <v>8.4000000000000005E-2</v>
-      </c>
-    </row>
-    <row r="58" spans="1:21">
-      <c r="A58" s="5"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="7"/>
-      <c r="J58" s="7">
-        <v>0.93</v>
-      </c>
-      <c r="L58" s="5">
-        <v>8.5999999999999993E-2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:21">
-      <c r="A59" s="5"/>
-      <c r="B59" s="7"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="7"/>
-      <c r="J59" s="7">
-        <v>0.93100000000000005</v>
-      </c>
-      <c r="L59" s="5">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="60" spans="1:21">
-      <c r="A60" s="5"/>
-      <c r="B60" s="7"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="7"/>
-      <c r="J60" s="7">
-        <v>0.93300000000000005</v>
-      </c>
-      <c r="L60" s="5">
-        <v>0.10199999999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:21">
-      <c r="A61" s="5"/>
-      <c r="B61" s="7"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="7"/>
-      <c r="J61" s="7">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="L61" s="5">
-        <v>0.106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:21">
-      <c r="A62" s="5"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="7"/>
-      <c r="J62" s="7">
-        <v>0.94</v>
-      </c>
-      <c r="L62" s="5">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="63" spans="1:21">
-      <c r="A63" s="5"/>
-      <c r="B63" s="7"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="7"/>
-      <c r="J63" s="7">
-        <v>0.94</v>
-      </c>
-      <c r="L63" s="5">
-        <v>0.115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:21">
-      <c r="A64" s="5"/>
-      <c r="B64" s="7"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="7"/>
-      <c r="J64" s="7">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="L64" s="5">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12">
-      <c r="A65" s="5"/>
-      <c r="B65" s="7"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="7"/>
-      <c r="J65" s="7">
-        <v>0.94399999999999995</v>
-      </c>
-      <c r="L65" s="5">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="5"/>
-      <c r="B66" s="7"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="7"/>
-      <c r="J66" s="7">
-        <v>0.94599999999999995</v>
-      </c>
-      <c r="L66" s="5">
-        <v>0.13</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
-      <c r="A67" s="5"/>
-      <c r="B67" s="7"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="7"/>
-      <c r="J67" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="L67" s="5">
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12">
-      <c r="A68" s="5"/>
-      <c r="B68" s="7"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="7"/>
-      <c r="J68" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="L68" s="5">
-        <v>0.14799999999999999</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
-      <c r="A69" s="5"/>
-      <c r="B69" s="7"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="7"/>
-      <c r="J69" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="L69" s="5">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12">
-      <c r="A70" s="5"/>
-      <c r="B70" s="7"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="7"/>
-      <c r="J70" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="L70" s="5">
-        <v>0.16300000000000001</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="A71" s="5"/>
-      <c r="B71" s="7"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="7"/>
-      <c r="J71" s="7">
-        <v>0.95</v>
-      </c>
-      <c r="L71" s="5">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="A72" s="5"/>
-      <c r="B72" s="7"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="7"/>
-      <c r="J72" s="7">
-        <v>0.96</v>
-      </c>
-      <c r="L72" s="5">
-        <v>0.17799999999999999</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="A73" s="5"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="7"/>
-      <c r="J73" s="7">
-        <v>0.96299999999999997</v>
-      </c>
-      <c r="L73" s="5">
-        <v>0.187</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12">
-      <c r="J74" s="7">
-        <v>0.96399999999999997</v>
-      </c>
-      <c r="L74" s="5">
-        <v>0.25</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState ref="L26:L74">
-    <sortCondition ref="L26"/>
-  </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>